<commit_message>
nuestro costo minimo y tiempo
agregado el costo minimo calculado por nosotros y el tiempo en milisegundos que nos da dicha operacion
</commit_message>
<xml_diff>
--- a/results-assignment.xlsx
+++ b/results-assignment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\NetBeansProjects\BinPackingProblem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Instaladores\Programacion\IDE\NetBeansProjects\BinPackingProblem-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="results-assignment" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="240">
   <si>
     <t>TIME</t>
   </si>
@@ -33,123 +33,258 @@
     <t xml:space="preserve">Filename </t>
   </si>
   <si>
+    <t>0.002588403</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.003325543</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.003637324</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.004368698</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.002038406</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.002007158</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>180.41</t>
+  </si>
+  <si>
+    <t>0.002225989</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.002256875</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.003035798</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.003299049</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT1_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.002386309</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.005397496</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.004053079</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.002676396</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.002573444</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.004663336</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.001774409</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>180.78</t>
+  </si>
+  <si>
+    <t>0.002363842</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>180.83</t>
+  </si>
+  <si>
+    <t>0.003050081</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.004070406</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV1_NT2_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.005146558</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.005427817</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.003911433</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.004455224</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.004002434</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.013272069</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.00523911</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>180.4</t>
+  </si>
+  <si>
+    <t>0.004660458</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.005965858</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.003852695</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT1_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>181.47</t>
+  </si>
+  <si>
+    <t>0.075161296</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.07738135</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.038542944</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.080557518</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.075439795</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.073316297</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.060666078</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.008860495</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.08337589</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.004082025</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT1000_ITV2_NT2_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
@@ -159,18 +294,30 @@
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.00005032</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.000079848</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.000079973</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.000057934</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
@@ -180,60 +327,105 @@
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>3.29</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT1_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.000098367</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.000091916</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.000087812</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.000094811</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.000091592</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.000052854</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV1_NT2_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>5.34</t>
+  </si>
+  <si>
+    <t>0.000047978</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.000091055</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>5.23</t>
+  </si>
+  <si>
+    <t>0.000048469</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.00008392</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.000099789</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.000099296</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
@@ -243,160 +435,310 @@
     <t>MPVSBPP_SET1_IT200_ITV2_NT1_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.000069125</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.000088849</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.000090086</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>13.17</t>
+  </si>
+  <si>
+    <t>0.000057353</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.000915952</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.000098432</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.000099892</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT200_ITV2_NT2_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.000026191</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.001070248</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.001110203</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.001196738</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.00056702</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.000041084</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.001213922</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.00007341</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.001676024</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT1_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.000086442</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.000099725</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.00142344</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.001550292</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.001484238</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.000066768</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>180.19</t>
+  </si>
+  <si>
+    <t>0.000318239</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.001288687</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.001570192</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.000575065</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV1_NT2_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.003879997</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.001478702</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.003824948</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.004425099</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.002052655</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.003381601</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>180.18</t>
+  </si>
+  <si>
+    <t>0.002916667</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.003673063</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.003774495</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.001988953</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT1_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
+    <t>0.002437159</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP1</t>
   </si>
   <si>
+    <t>0.005586301</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP10</t>
   </si>
   <si>
+    <t>0.001867249</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP2</t>
   </si>
   <si>
+    <t>0.002253253</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP3</t>
   </si>
   <si>
+    <t>0.001282299</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP4</t>
   </si>
   <si>
+    <t>0.001618667</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP5</t>
   </si>
   <si>
+    <t>0.002251269</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP6</t>
   </si>
   <si>
+    <t>0.002753275</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP7</t>
   </si>
   <si>
+    <t>0.002933029</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP8</t>
   </si>
   <si>
+    <t>0.004102163</t>
+  </si>
+  <si>
     <t>MPVSBPP_SET1_IT500_ITV2_NT2_TS3_WT1_VT1_REP9</t>
   </si>
   <si>
-    <t>My Solution</t>
-  </si>
-  <si>
-    <t>difference</t>
+    <t>MinimunCost</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Time (miliseconds)</t>
   </si>
 </sst>
 </file>
@@ -880,8 +1222,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1203,22 +1546,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1232,87 +1574,99 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>180.38300000000001</v>
+        <v>238</v>
+      </c>
+      <c r="H1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>180383</v>
       </c>
       <c r="B2">
         <v>96971</v>
       </c>
-      <c r="C2">
-        <v>2.588403E-3</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>96997</v>
       </c>
       <c r="G2">
-        <f>F2-B2</f>
+        <f t="shared" ref="G2:G66" si="0">F2-B2</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>180.38300000000001</v>
+      <c r="H2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>180383</v>
       </c>
       <c r="B3">
         <v>97127</v>
       </c>
-      <c r="C3">
-        <v>3.3255429999999998E-3</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>97081</v>
       </c>
       <c r="G3">
-        <f>F3-B3</f>
+        <f t="shared" si="0"/>
         <v>-46</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>180.40799999999999</v>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>180408</v>
       </c>
       <c r="B4">
         <v>98424</v>
       </c>
-      <c r="C4">
-        <v>3.6373239999999999E-3</v>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>98394</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G25" si="0">F4-B4</f>
+        <f t="shared" si="0"/>
         <v>-30</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>180.357</v>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>180357</v>
       </c>
       <c r="B5">
         <v>97283</v>
       </c>
-      <c r="C5">
-        <v>4.3686979999999999E-3</v>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>97123</v>
@@ -1321,19 +1675,22 @@
         <f t="shared" si="0"/>
         <v>-160</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>180.619</v>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>180619</v>
       </c>
       <c r="B6">
         <v>95663</v>
       </c>
-      <c r="C6">
-        <v>2.038406E-3</v>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>95791</v>
@@ -1342,19 +1699,22 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>180.559</v>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>180559</v>
       </c>
       <c r="B7">
         <v>94163</v>
       </c>
-      <c r="C7">
-        <v>2.0071580000000002E-3</v>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>94261</v>
@@ -1363,19 +1723,22 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>180.41</v>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
       </c>
       <c r="B8">
         <v>97934</v>
       </c>
-      <c r="C8">
-        <v>2.2259889999999998E-3</v>
+      <c r="C8" t="s">
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>97972</v>
@@ -1384,19 +1747,22 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>180.35400000000001</v>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>180354</v>
       </c>
       <c r="B9">
         <v>97923</v>
       </c>
-      <c r="C9">
-        <v>2.2568750000000002E-3</v>
+      <c r="C9" t="s">
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>97937</v>
@@ -1405,19 +1771,22 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>180.74600000000001</v>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>180746</v>
       </c>
       <c r="B10">
         <v>96515</v>
       </c>
-      <c r="C10">
-        <v>3.0357980000000001E-3</v>
+      <c r="C10" t="s">
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F10">
         <v>96591</v>
@@ -1426,19 +1795,22 @@
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>180.374</v>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>180374</v>
       </c>
       <c r="B11">
         <v>97907</v>
       </c>
-      <c r="C11">
-        <v>3.2990490000000001E-3</v>
+      <c r="C11" t="s">
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>97881</v>
@@ -1447,19 +1819,22 @@
         <f t="shared" si="0"/>
         <v>-26</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>495.10599999999999</v>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>495106</v>
       </c>
       <c r="B12">
         <v>95126</v>
       </c>
-      <c r="C12">
-        <v>2.3863090000000001E-3</v>
+      <c r="C12" t="s">
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>96696</v>
@@ -1468,19 +1843,22 @@
         <f t="shared" si="0"/>
         <v>1570</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>456.91199999999998</v>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>456912</v>
       </c>
       <c r="B13">
         <v>95674</v>
       </c>
-      <c r="C13">
-        <v>5.3974959999999999E-3</v>
+      <c r="C13" t="s">
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>96934</v>
@@ -1489,19 +1867,22 @@
         <f t="shared" si="0"/>
         <v>1260</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>436.62099999999998</v>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>436621</v>
       </c>
       <c r="B14">
         <v>95631</v>
       </c>
-      <c r="C14">
-        <v>4.0530790000000002E-3</v>
+      <c r="C14" t="s">
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>97011</v>
@@ -1510,19 +1891,22 @@
         <f t="shared" si="0"/>
         <v>1380</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>435.99799999999999</v>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>435998</v>
       </c>
       <c r="B15">
         <v>95651</v>
       </c>
-      <c r="C15">
-        <v>2.6763960000000002E-3</v>
+      <c r="C15" t="s">
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F15">
         <v>97151</v>
@@ -1531,19 +1915,22 @@
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>180.768</v>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>180768</v>
       </c>
       <c r="B16">
         <v>94970</v>
       </c>
-      <c r="C16">
-        <v>2.5734439999999998E-3</v>
+      <c r="C16" t="s">
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F16">
         <v>96570</v>
@@ -1552,19 +1939,22 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>180.881</v>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>180881</v>
       </c>
       <c r="B17">
         <v>96283</v>
       </c>
-      <c r="C17">
-        <v>4.6633359999999997E-3</v>
+      <c r="C17" t="s">
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F17">
         <v>97643</v>
@@ -1573,19 +1963,22 @@
         <f t="shared" si="0"/>
         <v>1360</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>376.91699999999997</v>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>376917</v>
       </c>
       <c r="B18">
         <v>95243</v>
       </c>
-      <c r="C18">
-        <v>1.774409E-3</v>
+      <c r="C18" t="s">
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F18">
         <v>96857</v>
@@ -1594,19 +1987,22 @@
         <f t="shared" si="0"/>
         <v>1614</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>180.78</v>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
       </c>
       <c r="B19">
         <v>94761</v>
       </c>
-      <c r="C19">
-        <v>2.3638420000000001E-3</v>
+      <c r="C19" t="s">
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>96281</v>
@@ -1615,19 +2011,22 @@
         <f t="shared" si="0"/>
         <v>1520</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>180.83</v>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
       </c>
       <c r="B20">
         <v>94227</v>
       </c>
-      <c r="C20">
-        <v>3.0500810000000001E-3</v>
+      <c r="C20" t="s">
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="F20">
         <v>95735</v>
@@ -1636,19 +2035,22 @@
         <f t="shared" si="0"/>
         <v>1508</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>432.16699999999997</v>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>432167</v>
       </c>
       <c r="B21">
         <v>95617</v>
       </c>
-      <c r="C21">
-        <v>4.0704060000000004E-3</v>
+      <c r="C21" t="s">
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F21">
         <v>96997</v>
@@ -1657,19 +2059,22 @@
         <f t="shared" si="0"/>
         <v>1380</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>180.39599999999999</v>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>180396</v>
       </c>
       <c r="B22">
         <v>117360</v>
       </c>
-      <c r="C22">
-        <v>5.1465579999999999E-3</v>
+      <c r="C22" t="s">
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F22">
         <v>117356</v>
@@ -1678,19 +2083,22 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>180.39500000000001</v>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>180395</v>
       </c>
       <c r="B23">
         <v>116253</v>
       </c>
-      <c r="C23">
-        <v>5.4278169999999997E-3</v>
+      <c r="C23" t="s">
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F23">
         <v>116183</v>
@@ -1699,19 +2107,22 @@
         <f t="shared" si="0"/>
         <v>-70</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>208.52699999999999</v>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>208527</v>
       </c>
       <c r="B24">
         <v>115303</v>
       </c>
-      <c r="C24">
-        <v>3.9114329999999998E-3</v>
+      <c r="C24" t="s">
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F24">
         <v>115397</v>
@@ -1720,19 +2131,22 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>180.517</v>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>180517</v>
       </c>
       <c r="B25">
         <v>116268</v>
       </c>
-      <c r="C25">
-        <v>4.4552239999999998E-3</v>
+      <c r="C25" t="s">
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F25">
         <v>116302</v>
@@ -1741,237 +2155,397 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>180.42699999999999</v>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>180427</v>
       </c>
       <c r="B26">
         <v>116679</v>
       </c>
-      <c r="C26">
-        <v>4.002434E-3</v>
+      <c r="C26" t="s">
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>180.47300000000001</v>
+        <v>56</v>
+      </c>
+      <c r="F26">
+        <v>116745</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>180473</v>
       </c>
       <c r="B27">
         <v>117088</v>
       </c>
-      <c r="C27">
-        <v>1.3272068999999999E-2</v>
+      <c r="C27" t="s">
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>180.452</v>
+        <v>58</v>
+      </c>
+      <c r="F27">
+        <v>116022</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>-1066</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>180452</v>
       </c>
       <c r="B28">
         <v>116432</v>
       </c>
-      <c r="C28">
-        <v>5.2391099999999999E-3</v>
+      <c r="C28" t="s">
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>180.4</v>
+        <v>60</v>
+      </c>
+      <c r="F28">
+        <v>116358</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>-74</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
       </c>
       <c r="B29">
         <v>116083</v>
       </c>
-      <c r="C29">
-        <v>4.6604580000000001E-3</v>
+      <c r="C29" t="s">
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>189.79400000000001</v>
+        <v>63</v>
+      </c>
+      <c r="F29">
+        <v>116113</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>189794</v>
       </c>
       <c r="B30">
         <v>116161</v>
       </c>
-      <c r="C30">
-        <v>5.9658580000000001E-3</v>
+      <c r="C30" t="s">
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>193.702</v>
+        <v>65</v>
+      </c>
+      <c r="F30">
+        <v>116043</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>-118</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>193702</v>
       </c>
       <c r="B31">
         <v>115244</v>
       </c>
-      <c r="C31">
-        <v>3.8526950000000002E-3</v>
+      <c r="C31" t="s">
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31">
-        <v>96857</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>181.47</v>
+        <v>67</v>
+      </c>
+      <c r="F31">
+        <v>115334</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>68</v>
       </c>
       <c r="B32">
         <v>123066</v>
       </c>
-      <c r="C32">
-        <v>7.5161296000000002E-2</v>
+      <c r="C32" t="s">
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>181.50700000000001</v>
+        <v>70</v>
+      </c>
+      <c r="F32">
+        <v>116148</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>-6918</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>181507</v>
       </c>
       <c r="B33">
         <v>122735</v>
       </c>
-      <c r="C33">
-        <v>7.7381350000000002E-2</v>
+      <c r="C33" t="s">
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>185.57499999999999</v>
+        <v>72</v>
+      </c>
+      <c r="F33">
+        <v>115509</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>-7226</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>185575</v>
       </c>
       <c r="B34">
         <v>118211</v>
       </c>
-      <c r="C34">
-        <v>3.8542944000000003E-2</v>
+      <c r="C34" t="s">
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>181.73599999999999</v>
+        <v>74</v>
+      </c>
+      <c r="F34">
+        <v>116015</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>-2196</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>181736</v>
       </c>
       <c r="B35">
         <v>124552</v>
       </c>
-      <c r="C35">
-        <v>8.0557517999999995E-2</v>
+      <c r="C35" t="s">
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>181.89500000000001</v>
+        <v>76</v>
+      </c>
+      <c r="F35">
+        <v>116892</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>-7660</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>181895</v>
       </c>
       <c r="B36">
         <v>121477</v>
       </c>
-      <c r="C36">
-        <v>7.5439795000000004E-2</v>
+      <c r="C36" t="s">
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>181.541</v>
+        <v>78</v>
+      </c>
+      <c r="F36">
+        <v>114583</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>-6894</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>181541</v>
       </c>
       <c r="B37">
         <v>122483</v>
       </c>
-      <c r="C37">
-        <v>7.3316297000000002E-2</v>
+      <c r="C37" t="s">
+        <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>181.541</v>
+        <v>80</v>
+      </c>
+      <c r="F37">
+        <v>115861</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>-6622</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>181541</v>
       </c>
       <c r="B38">
         <v>121277</v>
       </c>
-      <c r="C38">
-        <v>6.0666077999999998E-2</v>
+      <c r="C38" t="s">
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>184.23599999999999</v>
+        <v>82</v>
+      </c>
+      <c r="F38">
+        <v>116225</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>-5052</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>184236</v>
       </c>
       <c r="B39">
         <v>114892</v>
       </c>
-      <c r="C39">
-        <v>8.8604949999999995E-3</v>
+      <c r="C39" t="s">
+        <v>83</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>181.51499999999999</v>
+        <v>84</v>
+      </c>
+      <c r="F39">
+        <v>116190</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>1298</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>181515</v>
       </c>
       <c r="B40">
         <v>125324</v>
       </c>
-      <c r="C40">
-        <v>8.3375889999999994E-2</v>
+      <c r="C40" t="s">
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>181.428</v>
+        <v>86</v>
+      </c>
+      <c r="F40">
+        <v>117314</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>-8010</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>181428</v>
       </c>
       <c r="B41">
         <v>114502</v>
       </c>
-      <c r="C41">
-        <v>4.0820250000000004E-3</v>
+      <c r="C41" t="s">
+        <v>87</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2.3820000000000001</v>
+        <v>88</v>
+      </c>
+      <c r="F41">
+        <v>116344</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>1842</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>2382</v>
       </c>
       <c r="B42">
         <v>19874</v>
@@ -1980,12 +2554,22 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2.9079999999999999</v>
+        <v>89</v>
+      </c>
+      <c r="F42">
+        <v>19896</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>2908</v>
       </c>
       <c r="B43">
         <v>19812</v>
@@ -1994,54 +2578,94 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>9.7330000000000005</v>
+        <v>90</v>
+      </c>
+      <c r="F43">
+        <v>19854</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>9733</v>
       </c>
       <c r="B44">
         <v>19873</v>
       </c>
-      <c r="C44">
-        <v>5.0319999999999999E-5</v>
+      <c r="C44" t="s">
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>3.1509999999999998</v>
+        <v>92</v>
+      </c>
+      <c r="F44">
+        <v>19931</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>3151</v>
       </c>
       <c r="B45">
         <v>19154</v>
       </c>
-      <c r="C45">
-        <v>7.9847999999999999E-5</v>
+      <c r="C45" t="s">
+        <v>93</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>7.335</v>
+        <v>94</v>
+      </c>
+      <c r="F45">
+        <v>19194</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>7335</v>
       </c>
       <c r="B46">
         <v>19451</v>
       </c>
-      <c r="C46">
-        <v>7.9973000000000002E-5</v>
+      <c r="C46" t="s">
+        <v>95</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>3.0019999999999998</v>
+        <v>96</v>
+      </c>
+      <c r="F46">
+        <v>19495</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>3002</v>
       </c>
       <c r="B47">
         <v>19891</v>
@@ -2050,26 +2674,46 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>7.8860000000000001</v>
+        <v>97</v>
+      </c>
+      <c r="F47">
+        <v>19945</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>7886</v>
       </c>
       <c r="B48">
         <v>19179</v>
       </c>
-      <c r="C48">
-        <v>5.7933999999999998E-5</v>
+      <c r="C48" t="s">
+        <v>98</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>6.4770000000000003</v>
+        <v>99</v>
+      </c>
+      <c r="F48">
+        <v>19215</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>6477</v>
       </c>
       <c r="B49">
         <v>19350</v>
@@ -2078,12 +2722,22 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>14.147</v>
+        <v>100</v>
+      </c>
+      <c r="F49">
+        <v>19390</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>14147</v>
       </c>
       <c r="B50">
         <v>19156</v>
@@ -2092,12 +2746,22 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
+        <v>101</v>
+      </c>
+      <c r="F50">
+        <v>19208</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>3.29</v>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>102</v>
       </c>
       <c r="B51">
         <v>19781</v>
@@ -2106,12 +2770,22 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>7.3040000000000003</v>
+        <v>103</v>
+      </c>
+      <c r="F51">
+        <v>19833</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>7304</v>
       </c>
       <c r="B52">
         <v>19044</v>
@@ -2120,40 +2794,70 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>57.305999999999997</v>
+        <v>104</v>
+      </c>
+      <c r="F52">
+        <v>19404</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>57306</v>
       </c>
       <c r="B53">
         <v>19262</v>
       </c>
-      <c r="C53">
-        <v>9.8367000000000002E-5</v>
+      <c r="C53" t="s">
+        <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>13.885999999999999</v>
+        <v>106</v>
+      </c>
+      <c r="F53">
+        <v>19572</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>13886</v>
       </c>
       <c r="B54">
         <v>19711</v>
       </c>
-      <c r="C54">
-        <v>9.1916000000000006E-5</v>
+      <c r="C54" t="s">
+        <v>107</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>6.0490000000000004</v>
+        <v>108</v>
+      </c>
+      <c r="F54">
+        <v>20071</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>6049</v>
       </c>
       <c r="B55">
         <v>18835</v>
@@ -2162,26 +2866,46 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>8.7949999999999999</v>
+        <v>109</v>
+      </c>
+      <c r="F55">
+        <v>19215</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>8795</v>
       </c>
       <c r="B56">
         <v>18980</v>
       </c>
-      <c r="C56">
-        <v>8.7812000000000006E-5</v>
+      <c r="C56" t="s">
+        <v>110</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>6.7130000000000001</v>
+        <v>111</v>
+      </c>
+      <c r="F56">
+        <v>19320</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>6713</v>
       </c>
       <c r="B57">
         <v>19126</v>
@@ -2190,54 +2914,94 @@
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>20.402000000000001</v>
+        <v>112</v>
+      </c>
+      <c r="F57">
+        <v>19474</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>20402</v>
       </c>
       <c r="B58">
         <v>19276</v>
       </c>
-      <c r="C58">
-        <v>9.4810999999999997E-5</v>
+      <c r="C58" t="s">
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>8.1110000000000007</v>
+        <v>114</v>
+      </c>
+      <c r="F58">
+        <v>19586</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>8111</v>
       </c>
       <c r="B59">
         <v>19053</v>
       </c>
-      <c r="C59">
-        <v>9.1592E-5</v>
+      <c r="C59" t="s">
+        <v>115</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>18.295000000000002</v>
+        <v>116</v>
+      </c>
+      <c r="F59">
+        <v>19397</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>18295</v>
       </c>
       <c r="B60">
         <v>18920</v>
       </c>
-      <c r="C60">
-        <v>5.2853999999999999E-5</v>
+      <c r="C60" t="s">
+        <v>117</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>7.2770000000000001</v>
+        <v>118</v>
+      </c>
+      <c r="F60">
+        <v>19264</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>7277</v>
       </c>
       <c r="B61">
         <v>18758</v>
@@ -2246,26 +3010,46 @@
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>5.34</v>
+        <v>119</v>
+      </c>
+      <c r="F61">
+        <v>19138</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>120</v>
       </c>
       <c r="B62">
         <v>23159</v>
       </c>
-      <c r="C62">
-        <v>4.7978E-5</v>
+      <c r="C62" t="s">
+        <v>121</v>
       </c>
       <c r="D62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>5.3650000000000002</v>
+        <v>122</v>
+      </c>
+      <c r="F62">
+        <v>23257</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>5365</v>
       </c>
       <c r="B63">
         <v>23298</v>
@@ -2274,26 +3058,46 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>64.376999999999995</v>
+        <v>123</v>
+      </c>
+      <c r="F63">
+        <v>23390</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>64377</v>
       </c>
       <c r="B64">
         <v>23185</v>
       </c>
-      <c r="C64">
-        <v>9.1055000000000001E-5</v>
+      <c r="C64" t="s">
+        <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>4.6180000000000003</v>
+        <v>125</v>
+      </c>
+      <c r="F64">
+        <v>23299</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>4618</v>
       </c>
       <c r="B65">
         <v>22932</v>
@@ -2302,68 +3106,118 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>5.23</v>
+        <v>126</v>
+      </c>
+      <c r="F65">
+        <v>23040</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>127</v>
       </c>
       <c r="B66">
         <v>22924</v>
       </c>
-      <c r="C66">
-        <v>4.8469E-5</v>
+      <c r="C66" t="s">
+        <v>128</v>
       </c>
       <c r="D66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>22.373000000000001</v>
+        <v>129</v>
+      </c>
+      <c r="F66">
+        <v>23012</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>22373</v>
       </c>
       <c r="B67">
         <v>23034</v>
       </c>
-      <c r="C67">
-        <v>8.3919999999999996E-5</v>
+      <c r="C67" t="s">
+        <v>130</v>
       </c>
       <c r="D67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>18.475999999999999</v>
+        <v>131</v>
+      </c>
+      <c r="F67">
+        <v>23152</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G121" si="1">F67-B67</f>
+        <v>118</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>18476</v>
       </c>
       <c r="B68">
         <v>22826</v>
       </c>
-      <c r="C68">
-        <v>9.9789000000000003E-5</v>
+      <c r="C68" t="s">
+        <v>132</v>
       </c>
       <c r="D68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>22.724</v>
+        <v>133</v>
+      </c>
+      <c r="F68">
+        <v>22914</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>22724</v>
       </c>
       <c r="B69">
         <v>23322</v>
       </c>
-      <c r="C69">
-        <v>9.9296000000000006E-5</v>
+      <c r="C69" t="s">
+        <v>134</v>
       </c>
       <c r="D69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>5.8319999999999999</v>
+        <v>135</v>
+      </c>
+      <c r="F69">
+        <v>23418</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>5832</v>
       </c>
       <c r="B70">
         <v>22952</v>
@@ -2372,12 +3226,22 @@
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>6.5069999999999997</v>
+        <v>136</v>
+      </c>
+      <c r="F70">
+        <v>23054</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>6507</v>
       </c>
       <c r="B71">
         <v>23027</v>
@@ -2386,40 +3250,70 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>21.940999999999999</v>
+        <v>137</v>
+      </c>
+      <c r="F71">
+        <v>23117</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>21941</v>
       </c>
       <c r="B72">
         <v>22842</v>
       </c>
-      <c r="C72">
-        <v>6.9125E-5</v>
+      <c r="C72" t="s">
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>15.461</v>
+        <v>139</v>
+      </c>
+      <c r="F72">
+        <v>23292</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>15461</v>
       </c>
       <c r="B73">
         <v>22510</v>
       </c>
-      <c r="C73">
-        <v>8.8849000000000003E-5</v>
+      <c r="C73" t="s">
+        <v>140</v>
       </c>
       <c r="D73" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>12.694000000000001</v>
+        <v>141</v>
+      </c>
+      <c r="F73">
+        <v>23012</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="1"/>
+        <v>502</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>12694</v>
       </c>
       <c r="B74">
         <v>22947</v>
@@ -2428,54 +3322,94 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>12.792999999999999</v>
+        <v>142</v>
+      </c>
+      <c r="F74">
+        <v>23397</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>12793</v>
       </c>
       <c r="B75">
         <v>22201</v>
       </c>
-      <c r="C75">
-        <v>9.0086000000000005E-5</v>
+      <c r="C75" t="s">
+        <v>143</v>
       </c>
       <c r="D75" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>13.17</v>
+        <v>144</v>
+      </c>
+      <c r="F75">
+        <v>22639</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="1"/>
+        <v>438</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>145</v>
       </c>
       <c r="B76">
         <v>23248</v>
       </c>
-      <c r="C76">
-        <v>5.7352999999999998E-5</v>
+      <c r="C76" t="s">
+        <v>146</v>
       </c>
       <c r="D76" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>180.077</v>
+        <v>147</v>
+      </c>
+      <c r="F76">
+        <v>23770</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="1"/>
+        <v>522</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>180077</v>
       </c>
       <c r="B77">
         <v>22745</v>
       </c>
-      <c r="C77">
-        <v>9.1595200000000004E-4</v>
+      <c r="C77" t="s">
+        <v>148</v>
       </c>
       <c r="D77" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>12.617000000000001</v>
+        <v>149</v>
+      </c>
+      <c r="F77">
+        <v>23215</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="1"/>
+        <v>470</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>12617</v>
       </c>
       <c r="B78">
         <v>22975</v>
@@ -2484,40 +3418,70 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>17.449000000000002</v>
+        <v>150</v>
+      </c>
+      <c r="F78">
+        <v>23425</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>17449</v>
       </c>
       <c r="B79">
         <v>22470</v>
       </c>
-      <c r="C79">
-        <v>9.8431999999999995E-5</v>
+      <c r="C79" t="s">
+        <v>151</v>
       </c>
       <c r="D79" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>24.581</v>
+        <v>152</v>
+      </c>
+      <c r="F79">
+        <v>22970</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>24581</v>
       </c>
       <c r="B80">
         <v>23059</v>
       </c>
-      <c r="C80">
-        <v>9.9891999999999998E-5</v>
+      <c r="C80" t="s">
+        <v>153</v>
       </c>
       <c r="D80" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>10.109</v>
+        <v>154</v>
+      </c>
+      <c r="F80">
+        <v>23509</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>10109</v>
       </c>
       <c r="B81">
         <v>22503</v>
@@ -2526,96 +3490,166 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>46.521999999999998</v>
+        <v>155</v>
+      </c>
+      <c r="F81">
+        <v>22991</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>46522</v>
       </c>
       <c r="B82">
         <v>49410</v>
       </c>
-      <c r="C82">
-        <v>2.6191E-5</v>
+      <c r="C82" t="s">
+        <v>156</v>
       </c>
       <c r="D82" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>180.173</v>
+        <v>157</v>
+      </c>
+      <c r="F82">
+        <v>49556</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>180173</v>
       </c>
       <c r="B83">
         <v>48341</v>
       </c>
-      <c r="C83">
-        <v>1.070248E-3</v>
+      <c r="C83" t="s">
+        <v>158</v>
       </c>
       <c r="D83" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>180.11199999999999</v>
+        <v>159</v>
+      </c>
+      <c r="F83">
+        <v>48411</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>180112</v>
       </c>
       <c r="B84">
         <v>48940</v>
       </c>
-      <c r="C84">
-        <v>1.1102029999999999E-3</v>
+      <c r="C84" t="s">
+        <v>160</v>
       </c>
       <c r="D84" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>180.126</v>
+        <v>161</v>
+      </c>
+      <c r="F84">
+        <v>49092</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>180126</v>
       </c>
       <c r="B85">
         <v>48121</v>
       </c>
-      <c r="C85">
-        <v>1.1967379999999999E-3</v>
+      <c r="C85" t="s">
+        <v>162</v>
       </c>
       <c r="D85" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>180.12899999999999</v>
+        <v>163</v>
+      </c>
+      <c r="F85">
+        <v>48201</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>180129</v>
       </c>
       <c r="B86">
         <v>48162</v>
       </c>
-      <c r="C86">
-        <v>5.6702E-4</v>
+      <c r="C86" t="s">
+        <v>164</v>
       </c>
       <c r="D86" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>59.136000000000003</v>
+        <v>165</v>
+      </c>
+      <c r="F86">
+        <v>48264</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>59136</v>
       </c>
       <c r="B87">
         <v>48681</v>
       </c>
-      <c r="C87">
-        <v>4.1084000000000002E-5</v>
+      <c r="C87" t="s">
+        <v>166</v>
       </c>
       <c r="D87" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>58.485999999999997</v>
+        <v>167</v>
+      </c>
+      <c r="F87">
+        <v>48805</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>58486</v>
       </c>
       <c r="B88">
         <v>48680</v>
@@ -2624,475 +3658,812 @@
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>180.12299999999999</v>
+        <v>168</v>
+      </c>
+      <c r="F88">
+        <v>48784</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>180123</v>
       </c>
       <c r="B89">
         <v>47882</v>
       </c>
-      <c r="C89">
-        <v>1.2139220000000001E-3</v>
+      <c r="C89" t="s">
+        <v>169</v>
       </c>
       <c r="D89" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>34.267000000000003</v>
+        <v>170</v>
+      </c>
+      <c r="F89">
+        <v>47998</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>34267</v>
       </c>
       <c r="B90">
         <v>48178</v>
       </c>
-      <c r="C90">
-        <v>7.3410000000000004E-5</v>
+      <c r="C90" t="s">
+        <v>171</v>
       </c>
       <c r="D90" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>180.11799999999999</v>
+        <v>172</v>
+      </c>
+      <c r="F90">
+        <v>48278</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>180118</v>
       </c>
       <c r="B91">
         <v>47732</v>
       </c>
-      <c r="C91">
-        <v>1.6760239999999999E-3</v>
+      <c r="C91" t="s">
+        <v>173</v>
       </c>
       <c r="D91" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>146.10900000000001</v>
+        <v>174</v>
+      </c>
+      <c r="F91">
+        <v>47758</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>146109</v>
       </c>
       <c r="B92">
         <v>46274</v>
       </c>
-      <c r="C92">
-        <v>8.6441999999999997E-5</v>
+      <c r="C92" t="s">
+        <v>175</v>
       </c>
       <c r="D92" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>151.78399999999999</v>
+        <v>176</v>
+      </c>
+      <c r="F92">
+        <v>47156</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="1"/>
+        <v>882</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>151784</v>
       </c>
       <c r="B93">
         <v>47499</v>
       </c>
-      <c r="C93">
-        <v>9.9724999999999998E-5</v>
+      <c r="C93" t="s">
+        <v>177</v>
       </c>
       <c r="D93" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>180.18199999999999</v>
+        <v>178</v>
+      </c>
+      <c r="F93">
+        <v>48369</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>180182</v>
       </c>
       <c r="B94">
         <v>47180</v>
       </c>
-      <c r="C94">
-        <v>1.42344E-3</v>
+      <c r="C94" t="s">
+        <v>179</v>
       </c>
       <c r="D94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>180.209</v>
+        <v>180</v>
+      </c>
+      <c r="F94">
+        <v>48040</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="1"/>
+        <v>860</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>180209</v>
       </c>
       <c r="B95">
         <v>48636</v>
       </c>
-      <c r="C95">
-        <v>1.550292E-3</v>
+      <c r="C95" t="s">
+        <v>181</v>
       </c>
       <c r="D95" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>180.88900000000001</v>
+        <v>182</v>
+      </c>
+      <c r="F95">
+        <v>49556</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="1"/>
+        <v>920</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>180889</v>
       </c>
       <c r="B96">
         <v>48375</v>
       </c>
-      <c r="C96">
-        <v>1.4842379999999999E-3</v>
+      <c r="C96" t="s">
+        <v>183</v>
       </c>
       <c r="D96" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>139.649</v>
+        <v>184</v>
+      </c>
+      <c r="F96">
+        <v>49225</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="1"/>
+        <v>850</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>139649</v>
       </c>
       <c r="B97">
         <v>47927</v>
       </c>
-      <c r="C97">
-        <v>6.6767999999999995E-5</v>
+      <c r="C97" t="s">
+        <v>185</v>
       </c>
       <c r="D97" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>180.19</v>
+        <v>186</v>
+      </c>
+      <c r="F97">
+        <v>48847</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="1"/>
+        <v>920</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>187</v>
       </c>
       <c r="B98">
         <v>47920</v>
       </c>
-      <c r="C98">
-        <v>3.18239E-4</v>
+      <c r="C98" t="s">
+        <v>188</v>
       </c>
       <c r="D98" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>180.17400000000001</v>
+        <v>189</v>
+      </c>
+      <c r="F98">
+        <v>48840</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="1"/>
+        <v>920</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>180174</v>
       </c>
       <c r="B99">
         <v>48111</v>
       </c>
-      <c r="C99">
-        <v>1.2886869999999999E-3</v>
+      <c r="C99" t="s">
+        <v>190</v>
       </c>
       <c r="D99" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>180.154</v>
+        <v>191</v>
+      </c>
+      <c r="F99">
+        <v>48987</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="1"/>
+        <v>876</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>180154</v>
       </c>
       <c r="B100">
         <v>47128</v>
       </c>
-      <c r="C100">
-        <v>1.570192E-3</v>
+      <c r="C100" t="s">
+        <v>192</v>
       </c>
       <c r="D100" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>180.16300000000001</v>
+        <v>193</v>
+      </c>
+      <c r="F100">
+        <v>47998</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>180163</v>
       </c>
       <c r="B101">
         <v>47474</v>
       </c>
-      <c r="C101">
-        <v>5.7506500000000004E-4</v>
+      <c r="C101" t="s">
+        <v>194</v>
       </c>
       <c r="D101" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>180.14500000000001</v>
+        <v>195</v>
+      </c>
+      <c r="F101">
+        <v>48320</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="1"/>
+        <v>846</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>180145</v>
       </c>
       <c r="B102">
         <v>57732</v>
       </c>
-      <c r="C102">
-        <v>3.879997E-3</v>
+      <c r="C102" t="s">
+        <v>196</v>
       </c>
       <c r="D102" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>180.124</v>
+        <v>197</v>
+      </c>
+      <c r="F102">
+        <v>57808</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>180124</v>
       </c>
       <c r="B103">
         <v>57821</v>
       </c>
-      <c r="C103">
-        <v>1.4787019999999999E-3</v>
+      <c r="C103" t="s">
+        <v>198</v>
       </c>
       <c r="D103" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>180.226</v>
+        <v>199</v>
+      </c>
+      <c r="F103">
+        <v>57997</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>180226</v>
       </c>
       <c r="B104">
         <v>58040</v>
       </c>
-      <c r="C104">
-        <v>3.8249479999999999E-3</v>
+      <c r="C104" t="s">
+        <v>200</v>
       </c>
       <c r="D104" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>180.155</v>
+        <v>201</v>
+      </c>
+      <c r="F104">
+        <v>58046</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>180155</v>
       </c>
       <c r="B105">
         <v>58515</v>
       </c>
-      <c r="C105">
-        <v>4.425099E-3</v>
+      <c r="C105" t="s">
+        <v>202</v>
       </c>
       <c r="D105" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>180.08699999999999</v>
+        <v>203</v>
+      </c>
+      <c r="F105">
+        <v>58559</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>180087</v>
       </c>
       <c r="B106">
         <v>58216</v>
       </c>
-      <c r="C106">
-        <v>2.052655E-3</v>
+      <c r="C106" t="s">
+        <v>204</v>
       </c>
       <c r="D106" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>180.13300000000001</v>
+        <v>205</v>
+      </c>
+      <c r="F106">
+        <v>58384</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>180133</v>
       </c>
       <c r="B107">
         <v>57665</v>
       </c>
-      <c r="C107">
-        <v>3.3816010000000001E-3</v>
+      <c r="C107" t="s">
+        <v>206</v>
       </c>
       <c r="D107" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>180.18</v>
+        <v>207</v>
+      </c>
+      <c r="F107">
+        <v>57773</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>208</v>
       </c>
       <c r="B108">
         <v>57600</v>
       </c>
-      <c r="C108">
-        <v>2.916667E-3</v>
+      <c r="C108" t="s">
+        <v>209</v>
       </c>
       <c r="D108" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>180.14500000000001</v>
+        <v>210</v>
+      </c>
+      <c r="F108">
+        <v>57724</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>180145</v>
       </c>
       <c r="B109">
         <v>58262</v>
       </c>
-      <c r="C109">
-        <v>3.6730629999999998E-3</v>
+      <c r="C109" t="s">
+        <v>211</v>
       </c>
       <c r="D109" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>180.16300000000001</v>
+        <v>212</v>
+      </c>
+      <c r="F109">
+        <v>58370</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>180163</v>
       </c>
       <c r="B110">
         <v>58021</v>
       </c>
-      <c r="C110">
-        <v>3.7744950000000001E-3</v>
+      <c r="C110" t="s">
+        <v>213</v>
       </c>
       <c r="D110" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>180.19200000000001</v>
+        <v>214</v>
+      </c>
+      <c r="F110">
+        <v>58067</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>180192</v>
       </c>
       <c r="B111">
         <v>58385</v>
       </c>
-      <c r="C111">
-        <v>1.9889529999999999E-3</v>
+      <c r="C111" t="s">
+        <v>215</v>
       </c>
       <c r="D111" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>185.10499999999999</v>
+        <v>216</v>
+      </c>
+      <c r="F111">
+        <v>58573</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="1"/>
+        <v>188</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>185105</v>
       </c>
       <c r="B112">
         <v>57526</v>
       </c>
-      <c r="C112">
-        <v>2.4371589999999999E-3</v>
+      <c r="C112" t="s">
+        <v>217</v>
       </c>
       <c r="D112" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>180.34299999999999</v>
+        <v>218</v>
+      </c>
+      <c r="F112">
+        <v>58580</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="1"/>
+        <v>1054</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>180343</v>
       </c>
       <c r="B113">
         <v>57462</v>
       </c>
-      <c r="C113">
-        <v>5.5863010000000001E-3</v>
+      <c r="C113" t="s">
+        <v>219</v>
       </c>
       <c r="D113" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>180.22399999999999</v>
+        <v>220</v>
+      </c>
+      <c r="F113">
+        <v>58384</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="1"/>
+        <v>922</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>180224</v>
       </c>
       <c r="B114">
         <v>56768</v>
       </c>
-      <c r="C114">
-        <v>1.8672490000000001E-3</v>
+      <c r="C114" t="s">
+        <v>221</v>
       </c>
       <c r="D114" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>180.256</v>
+        <v>222</v>
+      </c>
+      <c r="F114">
+        <v>57864</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="1"/>
+        <v>1096</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>180256</v>
       </c>
       <c r="B115">
         <v>56718</v>
       </c>
-      <c r="C115">
-        <v>2.2532530000000002E-3</v>
+      <c r="C115" t="s">
+        <v>223</v>
       </c>
       <c r="D115" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>180.227</v>
+        <v>224</v>
+      </c>
+      <c r="F115">
+        <v>57766</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="1"/>
+        <v>1048</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>180227</v>
       </c>
       <c r="B116">
         <v>56968</v>
       </c>
-      <c r="C116">
-        <v>1.282299E-3</v>
+      <c r="C116" t="s">
+        <v>225</v>
       </c>
       <c r="D116" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>180.226</v>
+        <v>226</v>
+      </c>
+      <c r="F116">
+        <v>58060</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="1"/>
+        <v>1092</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>180226</v>
       </c>
       <c r="B117">
         <v>57084</v>
       </c>
-      <c r="C117">
-        <v>1.6186670000000001E-3</v>
+      <c r="C117" t="s">
+        <v>227</v>
       </c>
       <c r="D117" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>180.262</v>
+        <v>228</v>
+      </c>
+      <c r="F117">
+        <v>58144</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="1"/>
+        <v>1060</v>
+      </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>180262</v>
       </c>
       <c r="B118">
         <v>56557</v>
       </c>
-      <c r="C118">
-        <v>2.2512690000000002E-3</v>
+      <c r="C118" t="s">
+        <v>229</v>
       </c>
       <c r="D118" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>180.23699999999999</v>
+        <v>230</v>
+      </c>
+      <c r="F118">
+        <v>57647</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="1"/>
+        <v>1090</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>180237</v>
       </c>
       <c r="B119">
         <v>57023</v>
       </c>
-      <c r="C119">
-        <v>2.7532749999999999E-3</v>
+      <c r="C119" t="s">
+        <v>231</v>
       </c>
       <c r="D119" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>180.38800000000001</v>
+        <v>232</v>
+      </c>
+      <c r="F119">
+        <v>58053</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="1"/>
+        <v>1030</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>180388</v>
       </c>
       <c r="B120">
         <v>57756</v>
       </c>
-      <c r="C120">
-        <v>2.9330290000000002E-3</v>
+      <c r="C120" t="s">
+        <v>233</v>
       </c>
       <c r="D120" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>180.32300000000001</v>
+        <v>234</v>
+      </c>
+      <c r="F120">
+        <v>58776</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="1"/>
+        <v>1020</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>180323</v>
       </c>
       <c r="B121">
         <v>56263</v>
       </c>
-      <c r="C121">
-        <v>4.1021629999999998E-3</v>
+      <c r="C121" t="s">
+        <v>235</v>
       </c>
       <c r="D121" t="s">
-        <v>123</v>
+        <v>236</v>
+      </c>
+      <c r="F121">
+        <v>57183</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="1"/>
+        <v>920</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D121">
-    <sortCondition ref="D1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregadas librerias para gestionar Excel
</commit_message>
<xml_diff>
--- a/results-assignment.xlsx
+++ b/results-assignment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Addiel\Documents\GitHub\BinPackingProblem\"/>
     </mc:Choice>
@@ -751,6 +751,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1560,10 +1561,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="48.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.88671875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1608,15 +1609,15 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
-        <v>96997</v>
+      <c r="F2" t="n">
+        <v>96997.0</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G66" si="0">F2-B2</f>
         <v>26</v>
       </c>
-      <c r="H2">
-        <v>9</v>
+      <c r="H2" t="n">
+        <v>9.0</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I65" si="1">(F2-B2)/B2</f>
@@ -1640,15 +1641,15 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
-        <v>97081</v>
+      <c r="F3" t="n">
+        <v>97081.0</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
         <v>-46</v>
       </c>
-      <c r="H3">
-        <v>5</v>
+      <c r="H3" t="n">
+        <v>5.0</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
@@ -1672,15 +1673,15 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>98394</v>
+      <c r="F4" t="n">
+        <v>98394.0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
         <v>-30</v>
       </c>
-      <c r="H4">
-        <v>3</v>
+      <c r="H4" t="n">
+        <v>2.0</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
@@ -1704,15 +1705,15 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="F5">
-        <v>97123</v>
+      <c r="F5" t="n">
+        <v>97123.0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
         <v>-160</v>
       </c>
-      <c r="H5">
-        <v>2</v>
+      <c r="H5" t="n">
+        <v>2.0</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
@@ -1736,15 +1737,15 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="F6">
-        <v>95791</v>
+      <c r="F6" t="n">
+        <v>95791.0</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="H6">
-        <v>3</v>
+      <c r="H6" t="n">
+        <v>2.0</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
@@ -1768,15 +1769,15 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="F7">
-        <v>94261</v>
+      <c r="F7" t="n">
+        <v>94261.0</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="H7">
-        <v>2</v>
+      <c r="H7" t="n">
+        <v>1.0</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
@@ -1800,15 +1801,15 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="F8">
-        <v>97972</v>
+      <c r="F8" t="n">
+        <v>97972.0</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="H8">
-        <v>2</v>
+      <c r="H8" t="n">
+        <v>6.0</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
@@ -1832,15 +1833,15 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="F9">
-        <v>97937</v>
+      <c r="F9" t="n">
+        <v>97937.0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H9">
-        <v>1</v>
+      <c r="H9" t="n">
+        <v>1.0</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
@@ -1864,15 +1865,15 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="F10">
-        <v>96591</v>
+      <c r="F10" t="n">
+        <v>96591.0</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="H10">
-        <v>2</v>
+      <c r="H10" t="n">
+        <v>0.0</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
@@ -1896,15 +1897,15 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="F11">
-        <v>97881</v>
+      <c r="F11" t="n">
+        <v>97881.0</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
         <v>-26</v>
       </c>
-      <c r="H11">
-        <v>2</v>
+      <c r="H11" t="n">
+        <v>1.0</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
@@ -1928,15 +1929,15 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="F12">
-        <v>96696</v>
+      <c r="F12" t="n">
+        <v>96696.0</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>1570</v>
       </c>
-      <c r="H12">
-        <v>2</v>
+      <c r="H12" t="n">
+        <v>1.0</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
@@ -1960,15 +1961,15 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="F13">
-        <v>96934</v>
+      <c r="F13" t="n">
+        <v>96934.0</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
         <v>1260</v>
       </c>
-      <c r="H13">
-        <v>1</v>
+      <c r="H13" t="n">
+        <v>1.0</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
@@ -1992,15 +1993,15 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="F14">
-        <v>97011</v>
+      <c r="F14" t="n">
+        <v>97011.0</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
         <v>1380</v>
       </c>
-      <c r="H14">
-        <v>1</v>
+      <c r="H14" t="n">
+        <v>1.0</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
@@ -2024,15 +2025,15 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="F15">
-        <v>97151</v>
+      <c r="F15" t="n">
+        <v>97151.0</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="H15">
-        <v>2</v>
+      <c r="H15" t="n">
+        <v>1.0</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
@@ -2056,15 +2057,15 @@
       <c r="D16" t="s">
         <v>34</v>
       </c>
-      <c r="F16">
-        <v>96570</v>
+      <c r="F16" t="n">
+        <v>96570.0</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="H16">
-        <v>1</v>
+      <c r="H16" t="n">
+        <v>1.0</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
@@ -2088,15 +2089,15 @@
       <c r="D17" t="s">
         <v>36</v>
       </c>
-      <c r="F17">
-        <v>97643</v>
+      <c r="F17" t="n">
+        <v>97643.0</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
         <v>1360</v>
       </c>
-      <c r="H17">
-        <v>1</v>
+      <c r="H17" t="n">
+        <v>2.0</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
@@ -2120,15 +2121,15 @@
       <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="F18">
-        <v>96857</v>
+      <c r="F18" t="n">
+        <v>96857.0</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
         <v>1614</v>
       </c>
-      <c r="H18">
-        <v>0</v>
+      <c r="H18" t="n">
+        <v>1.0</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
@@ -2152,15 +2153,15 @@
       <c r="D19" t="s">
         <v>41</v>
       </c>
-      <c r="F19">
-        <v>96281</v>
+      <c r="F19" t="n">
+        <v>96281.0</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
         <v>1520</v>
       </c>
-      <c r="H19">
-        <v>1</v>
+      <c r="H19" t="n">
+        <v>1.0</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
@@ -2184,15 +2185,15 @@
       <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="F20">
-        <v>95735</v>
+      <c r="F20" t="n">
+        <v>95735.0</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
         <v>1508</v>
       </c>
-      <c r="H20">
-        <v>0</v>
+      <c r="H20" t="n">
+        <v>1.0</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
@@ -2216,15 +2217,15 @@
       <c r="D21" t="s">
         <v>46</v>
       </c>
-      <c r="F21">
-        <v>96997</v>
+      <c r="F21" t="n">
+        <v>96997.0</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
         <v>1380</v>
       </c>
-      <c r="H21">
-        <v>1</v>
+      <c r="H21" t="n">
+        <v>2.0</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
@@ -2248,15 +2249,15 @@
       <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="F22">
-        <v>117356</v>
+      <c r="F22" t="n">
+        <v>117356.0</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-      <c r="H22">
-        <v>1</v>
+      <c r="H22" t="n">
+        <v>1.0</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
@@ -2280,15 +2281,15 @@
       <c r="D23" t="s">
         <v>50</v>
       </c>
-      <c r="F23">
-        <v>116183</v>
+      <c r="F23" t="n">
+        <v>116183.0</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
         <v>-70</v>
       </c>
-      <c r="H23">
-        <v>1</v>
+      <c r="H23" t="n">
+        <v>1.0</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
@@ -2312,15 +2313,15 @@
       <c r="D24" t="s">
         <v>52</v>
       </c>
-      <c r="F24">
-        <v>115397</v>
+      <c r="F24" t="n">
+        <v>115397.0</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="H24">
-        <v>1</v>
+      <c r="H24" t="n">
+        <v>0.0</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
@@ -2344,15 +2345,15 @@
       <c r="D25" t="s">
         <v>54</v>
       </c>
-      <c r="F25">
-        <v>116302</v>
+      <c r="F25" t="n">
+        <v>116302.0</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H25">
-        <v>1</v>
+      <c r="H25" t="n">
+        <v>1.0</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
@@ -2376,15 +2377,15 @@
       <c r="D26" t="s">
         <v>56</v>
       </c>
-      <c r="F26">
-        <v>116745</v>
+      <c r="F26" t="n">
+        <v>116745.0</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="H26">
-        <v>1</v>
+      <c r="H26" t="n">
+        <v>0.0</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
@@ -2408,15 +2409,15 @@
       <c r="D27" t="s">
         <v>58</v>
       </c>
-      <c r="F27">
-        <v>116022</v>
+      <c r="F27" t="n">
+        <v>116022.0</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
         <v>-1066</v>
       </c>
-      <c r="H27">
-        <v>1</v>
+      <c r="H27" t="n">
+        <v>0.0</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
@@ -2440,15 +2441,15 @@
       <c r="D28" t="s">
         <v>60</v>
       </c>
-      <c r="F28">
-        <v>116358</v>
+      <c r="F28" t="n">
+        <v>116358.0</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
         <v>-74</v>
       </c>
-      <c r="H28">
-        <v>1</v>
+      <c r="H28" t="n">
+        <v>1.0</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
@@ -2472,15 +2473,15 @@
       <c r="D29" t="s">
         <v>63</v>
       </c>
-      <c r="F29">
-        <v>116113</v>
+      <c r="F29" t="n">
+        <v>116113.0</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H29">
-        <v>1</v>
+      <c r="H29" t="n">
+        <v>1.0</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
@@ -2504,15 +2505,15 @@
       <c r="D30" t="s">
         <v>65</v>
       </c>
-      <c r="F30">
-        <v>116043</v>
+      <c r="F30" t="n">
+        <v>116043.0</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
         <v>-118</v>
       </c>
-      <c r="H30">
-        <v>0</v>
+      <c r="H30" t="n">
+        <v>1.0</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
@@ -2536,15 +2537,15 @@
       <c r="D31" t="s">
         <v>67</v>
       </c>
-      <c r="F31">
-        <v>115334</v>
+      <c r="F31" t="n">
+        <v>115334.0</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H31">
-        <v>1</v>
+      <c r="H31" t="n">
+        <v>2.0</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
@@ -2568,15 +2569,15 @@
       <c r="D32" t="s">
         <v>70</v>
       </c>
-      <c r="F32">
-        <v>116148</v>
+      <c r="F32" t="n">
+        <v>116148.0</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
         <v>-6918</v>
       </c>
-      <c r="H32">
-        <v>1</v>
+      <c r="H32" t="n">
+        <v>0.0</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
@@ -2600,15 +2601,15 @@
       <c r="D33" t="s">
         <v>72</v>
       </c>
-      <c r="F33">
-        <v>115509</v>
+      <c r="F33" t="n">
+        <v>115509.0</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
         <v>-7226</v>
       </c>
-      <c r="H33">
-        <v>1</v>
+      <c r="H33" t="n">
+        <v>2.0</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
@@ -2632,15 +2633,15 @@
       <c r="D34" t="s">
         <v>74</v>
       </c>
-      <c r="F34">
-        <v>116015</v>
+      <c r="F34" t="n">
+        <v>116015.0</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
         <v>-2196</v>
       </c>
-      <c r="H34">
-        <v>1</v>
+      <c r="H34" t="n">
+        <v>1.0</v>
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
@@ -2664,15 +2665,15 @@
       <c r="D35" t="s">
         <v>76</v>
       </c>
-      <c r="F35">
-        <v>116892</v>
+      <c r="F35" t="n">
+        <v>116892.0</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
         <v>-7660</v>
       </c>
-      <c r="H35">
-        <v>1</v>
+      <c r="H35" t="n">
+        <v>1.0</v>
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
@@ -2696,15 +2697,15 @@
       <c r="D36" t="s">
         <v>78</v>
       </c>
-      <c r="F36">
-        <v>114583</v>
+      <c r="F36" t="n">
+        <v>114583.0</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
         <v>-6894</v>
       </c>
-      <c r="H36">
-        <v>2</v>
+      <c r="H36" t="n">
+        <v>0.0</v>
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
@@ -2728,15 +2729,15 @@
       <c r="D37" t="s">
         <v>80</v>
       </c>
-      <c r="F37">
-        <v>115861</v>
+      <c r="F37" t="n">
+        <v>115861.0</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
         <v>-6622</v>
       </c>
-      <c r="H37">
-        <v>0</v>
+      <c r="H37" t="n">
+        <v>1.0</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
@@ -2760,15 +2761,15 @@
       <c r="D38" t="s">
         <v>82</v>
       </c>
-      <c r="F38">
-        <v>116225</v>
+      <c r="F38" t="n">
+        <v>116225.0</v>
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
         <v>-5052</v>
       </c>
-      <c r="H38">
-        <v>2</v>
+      <c r="H38" t="n">
+        <v>1.0</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
@@ -2792,15 +2793,15 @@
       <c r="D39" t="s">
         <v>84</v>
       </c>
-      <c r="F39">
-        <v>116190</v>
+      <c r="F39" t="n">
+        <v>116190.0</v>
       </c>
       <c r="G39">
         <f t="shared" si="0"/>
         <v>1298</v>
       </c>
-      <c r="H39">
-        <v>1</v>
+      <c r="H39" t="n">
+        <v>1.0</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
@@ -2824,15 +2825,15 @@
       <c r="D40" t="s">
         <v>86</v>
       </c>
-      <c r="F40">
-        <v>117314</v>
+      <c r="F40" t="n">
+        <v>117314.0</v>
       </c>
       <c r="G40">
         <f t="shared" si="0"/>
         <v>-8010</v>
       </c>
-      <c r="H40">
-        <v>1</v>
+      <c r="H40" t="n">
+        <v>1.0</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
@@ -2856,15 +2857,15 @@
       <c r="D41" t="s">
         <v>88</v>
       </c>
-      <c r="F41">
-        <v>116344</v>
+      <c r="F41" t="n">
+        <v>116344.0</v>
       </c>
       <c r="G41">
         <f t="shared" si="0"/>
         <v>1842</v>
       </c>
-      <c r="H41">
-        <v>1</v>
+      <c r="H41" t="n">
+        <v>1.0</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
@@ -2888,15 +2889,15 @@
       <c r="D42" t="s">
         <v>89</v>
       </c>
-      <c r="F42">
-        <v>19896</v>
+      <c r="F42" t="n">
+        <v>19896.0</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H42">
-        <v>0</v>
+      <c r="H42" t="n">
+        <v>0.0</v>
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
@@ -2920,15 +2921,15 @@
       <c r="D43" t="s">
         <v>90</v>
       </c>
-      <c r="F43">
-        <v>19854</v>
+      <c r="F43" t="n">
+        <v>19854.0</v>
       </c>
       <c r="G43">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="H43">
-        <v>0</v>
+      <c r="H43" t="n">
+        <v>0.0</v>
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
@@ -2952,15 +2953,15 @@
       <c r="D44" t="s">
         <v>92</v>
       </c>
-      <c r="F44">
-        <v>19931</v>
+      <c r="F44" t="n">
+        <v>19931.0</v>
       </c>
       <c r="G44">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="H44">
-        <v>0</v>
+      <c r="H44" t="n">
+        <v>0.0</v>
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
@@ -2984,15 +2985,15 @@
       <c r="D45" t="s">
         <v>94</v>
       </c>
-      <c r="F45">
-        <v>19194</v>
+      <c r="F45" t="n">
+        <v>19194.0</v>
       </c>
       <c r="G45">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H45">
-        <v>0</v>
+      <c r="H45" t="n">
+        <v>0.0</v>
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
@@ -3016,15 +3017,15 @@
       <c r="D46" t="s">
         <v>96</v>
       </c>
-      <c r="F46">
-        <v>19495</v>
+      <c r="F46" t="n">
+        <v>19495.0</v>
       </c>
       <c r="G46">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="H46">
-        <v>0</v>
+      <c r="H46" t="n">
+        <v>0.0</v>
       </c>
       <c r="I46">
         <f t="shared" si="1"/>
@@ -3048,15 +3049,15 @@
       <c r="D47" t="s">
         <v>97</v>
       </c>
-      <c r="F47">
-        <v>19945</v>
+      <c r="F47" t="n">
+        <v>19945.0</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="H47">
-        <v>0</v>
+      <c r="H47" t="n">
+        <v>0.0</v>
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
@@ -3080,15 +3081,15 @@
       <c r="D48" t="s">
         <v>99</v>
       </c>
-      <c r="F48">
-        <v>19215</v>
+      <c r="F48" t="n">
+        <v>19215.0</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="H48">
-        <v>0</v>
+      <c r="H48" t="n">
+        <v>0.0</v>
       </c>
       <c r="I48">
         <f t="shared" si="1"/>
@@ -3112,15 +3113,15 @@
       <c r="D49" t="s">
         <v>100</v>
       </c>
-      <c r="F49">
-        <v>19390</v>
+      <c r="F49" t="n">
+        <v>19390.0</v>
       </c>
       <c r="G49">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H49">
-        <v>0</v>
+      <c r="H49" t="n">
+        <v>0.0</v>
       </c>
       <c r="I49">
         <f t="shared" si="1"/>
@@ -3144,15 +3145,15 @@
       <c r="D50" t="s">
         <v>101</v>
       </c>
-      <c r="F50">
-        <v>19208</v>
+      <c r="F50" t="n">
+        <v>19208.0</v>
       </c>
       <c r="G50">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="H50">
-        <v>1</v>
+      <c r="H50" t="n">
+        <v>1.0</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
@@ -3176,15 +3177,15 @@
       <c r="D51" t="s">
         <v>103</v>
       </c>
-      <c r="F51">
-        <v>19833</v>
+      <c r="F51" t="n">
+        <v>19833.0</v>
       </c>
       <c r="G51">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="H51">
-        <v>0</v>
+      <c r="H51" t="n">
+        <v>0.0</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
@@ -3208,15 +3209,15 @@
       <c r="D52" t="s">
         <v>104</v>
       </c>
-      <c r="F52">
-        <v>19404</v>
+      <c r="F52" t="n">
+        <v>19404.0</v>
       </c>
       <c r="G52">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="H52">
-        <v>0</v>
+      <c r="H52" t="n">
+        <v>1.0</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
@@ -3240,15 +3241,15 @@
       <c r="D53" t="s">
         <v>106</v>
       </c>
-      <c r="F53">
-        <v>19572</v>
+      <c r="F53" t="n">
+        <v>19572.0</v>
       </c>
       <c r="G53">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
-      <c r="H53">
-        <v>0</v>
+      <c r="H53" t="n">
+        <v>0.0</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
@@ -3272,15 +3273,15 @@
       <c r="D54" t="s">
         <v>108</v>
       </c>
-      <c r="F54">
-        <v>20071</v>
+      <c r="F54" t="n">
+        <v>20071.0</v>
       </c>
       <c r="G54">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="H54">
-        <v>0</v>
+      <c r="H54" t="n">
+        <v>1.0</v>
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
@@ -3304,15 +3305,15 @@
       <c r="D55" t="s">
         <v>109</v>
       </c>
-      <c r="F55">
-        <v>19215</v>
+      <c r="F55" t="n">
+        <v>19215.0</v>
       </c>
       <c r="G55">
         <f t="shared" si="0"/>
         <v>380</v>
       </c>
-      <c r="H55">
-        <v>0</v>
+      <c r="H55" t="n">
+        <v>1.0</v>
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
@@ -3336,15 +3337,15 @@
       <c r="D56" t="s">
         <v>111</v>
       </c>
-      <c r="F56">
-        <v>19320</v>
+      <c r="F56" t="n">
+        <v>19320.0</v>
       </c>
       <c r="G56">
         <f t="shared" si="0"/>
         <v>340</v>
       </c>
-      <c r="H56">
-        <v>0</v>
+      <c r="H56" t="n">
+        <v>0.0</v>
       </c>
       <c r="I56">
         <f t="shared" si="1"/>
@@ -3368,15 +3369,15 @@
       <c r="D57" t="s">
         <v>112</v>
       </c>
-      <c r="F57">
-        <v>19474</v>
+      <c r="F57" t="n">
+        <v>19474.0</v>
       </c>
       <c r="G57">
         <f t="shared" si="0"/>
         <v>348</v>
       </c>
-      <c r="H57">
-        <v>0</v>
+      <c r="H57" t="n">
+        <v>0.0</v>
       </c>
       <c r="I57">
         <f t="shared" si="1"/>
@@ -3400,15 +3401,15 @@
       <c r="D58" t="s">
         <v>114</v>
       </c>
-      <c r="F58">
-        <v>19586</v>
+      <c r="F58" t="n">
+        <v>19586.0</v>
       </c>
       <c r="G58">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
-      <c r="H58">
-        <v>0</v>
+      <c r="H58" t="n">
+        <v>0.0</v>
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
@@ -3432,15 +3433,15 @@
       <c r="D59" t="s">
         <v>116</v>
       </c>
-      <c r="F59">
-        <v>19397</v>
+      <c r="F59" t="n">
+        <v>19397.0</v>
       </c>
       <c r="G59">
         <f t="shared" si="0"/>
         <v>344</v>
       </c>
-      <c r="H59">
-        <v>0</v>
+      <c r="H59" t="n">
+        <v>1.0</v>
       </c>
       <c r="I59">
         <f t="shared" si="1"/>
@@ -3464,15 +3465,15 @@
       <c r="D60" t="s">
         <v>118</v>
       </c>
-      <c r="F60">
-        <v>19264</v>
+      <c r="F60" t="n">
+        <v>19264.0</v>
       </c>
       <c r="G60">
         <f t="shared" si="0"/>
         <v>344</v>
       </c>
-      <c r="H60">
-        <v>0</v>
+      <c r="H60" t="n">
+        <v>0.0</v>
       </c>
       <c r="I60">
         <f t="shared" si="1"/>
@@ -3496,15 +3497,15 @@
       <c r="D61" t="s">
         <v>119</v>
       </c>
-      <c r="F61">
-        <v>19138</v>
+      <c r="F61" t="n">
+        <v>19138.0</v>
       </c>
       <c r="G61">
         <f t="shared" si="0"/>
         <v>380</v>
       </c>
-      <c r="H61">
-        <v>0</v>
+      <c r="H61" t="n">
+        <v>0.0</v>
       </c>
       <c r="I61">
         <f t="shared" si="1"/>
@@ -3528,15 +3529,15 @@
       <c r="D62" t="s">
         <v>122</v>
       </c>
-      <c r="F62">
-        <v>23257</v>
+      <c r="F62" t="n">
+        <v>23257.0</v>
       </c>
       <c r="G62">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="H62">
-        <v>0</v>
+      <c r="H62" t="n">
+        <v>0.0</v>
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
@@ -3560,15 +3561,15 @@
       <c r="D63" t="s">
         <v>123</v>
       </c>
-      <c r="F63">
-        <v>23390</v>
+      <c r="F63" t="n">
+        <v>23390.0</v>
       </c>
       <c r="G63">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="H63">
-        <v>0</v>
+      <c r="H63" t="n">
+        <v>0.0</v>
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
@@ -3592,15 +3593,15 @@
       <c r="D64" t="s">
         <v>125</v>
       </c>
-      <c r="F64">
-        <v>23299</v>
+      <c r="F64" t="n">
+        <v>23299.0</v>
       </c>
       <c r="G64">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="H64">
-        <v>0</v>
+      <c r="H64" t="n">
+        <v>0.0</v>
       </c>
       <c r="I64">
         <f t="shared" si="1"/>
@@ -3624,15 +3625,15 @@
       <c r="D65" t="s">
         <v>126</v>
       </c>
-      <c r="F65">
-        <v>23040</v>
+      <c r="F65" t="n">
+        <v>23040.0</v>
       </c>
       <c r="G65">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="H65">
-        <v>0</v>
+      <c r="H65" t="n">
+        <v>0.0</v>
       </c>
       <c r="I65">
         <f t="shared" si="1"/>
@@ -3656,15 +3657,15 @@
       <c r="D66" t="s">
         <v>129</v>
       </c>
-      <c r="F66">
-        <v>23012</v>
+      <c r="F66" t="n">
+        <v>23012.0</v>
       </c>
       <c r="G66">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="H66">
-        <v>1</v>
+      <c r="H66" t="n">
+        <v>0.0</v>
       </c>
       <c r="I66">
         <f t="shared" ref="I66:I121" si="3">(F66-B66)/B66</f>
@@ -3688,15 +3689,15 @@
       <c r="D67" t="s">
         <v>131</v>
       </c>
-      <c r="F67">
-        <v>23152</v>
+      <c r="F67" t="n">
+        <v>23152.0</v>
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G121" si="4">F67-B67</f>
         <v>118</v>
       </c>
-      <c r="H67">
-        <v>0</v>
+      <c r="H67" t="n">
+        <v>0.0</v>
       </c>
       <c r="I67">
         <f t="shared" si="3"/>
@@ -3720,15 +3721,15 @@
       <c r="D68" t="s">
         <v>133</v>
       </c>
-      <c r="F68">
-        <v>22914</v>
+      <c r="F68" t="n">
+        <v>22914.0</v>
       </c>
       <c r="G68">
         <f t="shared" si="4"/>
         <v>88</v>
       </c>
-      <c r="H68">
-        <v>0</v>
+      <c r="H68" t="n">
+        <v>1.0</v>
       </c>
       <c r="I68">
         <f t="shared" si="3"/>
@@ -3752,15 +3753,15 @@
       <c r="D69" t="s">
         <v>135</v>
       </c>
-      <c r="F69">
-        <v>23418</v>
+      <c r="F69" t="n">
+        <v>23418.0</v>
       </c>
       <c r="G69">
         <f t="shared" si="4"/>
         <v>96</v>
       </c>
-      <c r="H69">
-        <v>0</v>
+      <c r="H69" t="n">
+        <v>1.0</v>
       </c>
       <c r="I69">
         <f t="shared" si="3"/>
@@ -3784,15 +3785,15 @@
       <c r="D70" t="s">
         <v>136</v>
       </c>
-      <c r="F70">
-        <v>23054</v>
+      <c r="F70" t="n">
+        <v>23054.0</v>
       </c>
       <c r="G70">
         <f t="shared" si="4"/>
         <v>102</v>
       </c>
-      <c r="H70">
-        <v>0</v>
+      <c r="H70" t="n">
+        <v>0.0</v>
       </c>
       <c r="I70">
         <f t="shared" si="3"/>
@@ -3816,15 +3817,15 @@
       <c r="D71" t="s">
         <v>137</v>
       </c>
-      <c r="F71">
-        <v>23117</v>
+      <c r="F71" t="n">
+        <v>23117.0</v>
       </c>
       <c r="G71">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="H71">
-        <v>0</v>
+      <c r="H71" t="n">
+        <v>0.0</v>
       </c>
       <c r="I71">
         <f t="shared" si="3"/>
@@ -3848,15 +3849,15 @@
       <c r="D72" t="s">
         <v>139</v>
       </c>
-      <c r="F72">
-        <v>23292</v>
+      <c r="F72" t="n">
+        <v>23292.0</v>
       </c>
       <c r="G72">
         <f t="shared" si="4"/>
         <v>450</v>
       </c>
-      <c r="H72">
-        <v>0</v>
+      <c r="H72" t="n">
+        <v>0.0</v>
       </c>
       <c r="I72">
         <f t="shared" si="3"/>
@@ -3880,15 +3881,15 @@
       <c r="D73" t="s">
         <v>141</v>
       </c>
-      <c r="F73">
-        <v>23012</v>
+      <c r="F73" t="n">
+        <v>23012.0</v>
       </c>
       <c r="G73">
         <f t="shared" si="4"/>
         <v>502</v>
       </c>
-      <c r="H73">
-        <v>0</v>
+      <c r="H73" t="n">
+        <v>0.0</v>
       </c>
       <c r="I73">
         <f t="shared" si="3"/>
@@ -3912,15 +3913,15 @@
       <c r="D74" t="s">
         <v>142</v>
       </c>
-      <c r="F74">
-        <v>23397</v>
+      <c r="F74" t="n">
+        <v>23397.0</v>
       </c>
       <c r="G74">
         <f t="shared" si="4"/>
         <v>450</v>
       </c>
-      <c r="H74">
-        <v>0</v>
+      <c r="H74" t="n">
+        <v>0.0</v>
       </c>
       <c r="I74">
         <f t="shared" si="3"/>
@@ -3944,15 +3945,15 @@
       <c r="D75" t="s">
         <v>144</v>
       </c>
-      <c r="F75">
-        <v>22639</v>
+      <c r="F75" t="n">
+        <v>22639.0</v>
       </c>
       <c r="G75">
         <f t="shared" si="4"/>
         <v>438</v>
       </c>
-      <c r="H75">
-        <v>0</v>
+      <c r="H75" t="n">
+        <v>0.0</v>
       </c>
       <c r="I75">
         <f t="shared" si="3"/>
@@ -3976,15 +3977,15 @@
       <c r="D76" t="s">
         <v>147</v>
       </c>
-      <c r="F76">
-        <v>23770</v>
+      <c r="F76" t="n">
+        <v>23770.0</v>
       </c>
       <c r="G76">
         <f t="shared" si="4"/>
         <v>522</v>
       </c>
-      <c r="H76">
-        <v>0</v>
+      <c r="H76" t="n">
+        <v>0.0</v>
       </c>
       <c r="I76">
         <f t="shared" si="3"/>
@@ -4008,15 +4009,15 @@
       <c r="D77" t="s">
         <v>149</v>
       </c>
-      <c r="F77">
-        <v>23215</v>
+      <c r="F77" t="n">
+        <v>23215.0</v>
       </c>
       <c r="G77">
         <f t="shared" si="4"/>
         <v>470</v>
       </c>
-      <c r="H77">
-        <v>0</v>
+      <c r="H77" t="n">
+        <v>0.0</v>
       </c>
       <c r="I77">
         <f t="shared" si="3"/>
@@ -4040,15 +4041,15 @@
       <c r="D78" t="s">
         <v>150</v>
       </c>
-      <c r="F78">
-        <v>23425</v>
+      <c r="F78" t="n">
+        <v>23425.0</v>
       </c>
       <c r="G78">
         <f t="shared" si="4"/>
         <v>450</v>
       </c>
-      <c r="H78">
-        <v>0</v>
+      <c r="H78" t="n">
+        <v>1.0</v>
       </c>
       <c r="I78">
         <f t="shared" si="3"/>
@@ -4072,15 +4073,15 @@
       <c r="D79" t="s">
         <v>152</v>
       </c>
-      <c r="F79">
-        <v>22970</v>
+      <c r="F79" t="n">
+        <v>22970.0</v>
       </c>
       <c r="G79">
         <f t="shared" si="4"/>
         <v>500</v>
       </c>
-      <c r="H79">
-        <v>0</v>
+      <c r="H79" t="n">
+        <v>0.0</v>
       </c>
       <c r="I79">
         <f t="shared" si="3"/>
@@ -4104,15 +4105,15 @@
       <c r="D80" t="s">
         <v>154</v>
       </c>
-      <c r="F80">
-        <v>23509</v>
+      <c r="F80" t="n">
+        <v>23509.0</v>
       </c>
       <c r="G80">
         <f t="shared" si="4"/>
         <v>450</v>
       </c>
-      <c r="H80">
-        <v>0</v>
+      <c r="H80" t="n">
+        <v>0.0</v>
       </c>
       <c r="I80">
         <f t="shared" si="3"/>
@@ -4136,15 +4137,15 @@
       <c r="D81" t="s">
         <v>155</v>
       </c>
-      <c r="F81">
-        <v>22991</v>
+      <c r="F81" t="n">
+        <v>22991.0</v>
       </c>
       <c r="G81">
         <f t="shared" si="4"/>
         <v>488</v>
       </c>
-      <c r="H81">
-        <v>1</v>
+      <c r="H81" t="n">
+        <v>0.0</v>
       </c>
       <c r="I81">
         <f t="shared" si="3"/>
@@ -4168,15 +4169,15 @@
       <c r="D82" t="s">
         <v>157</v>
       </c>
-      <c r="F82">
-        <v>49556</v>
+      <c r="F82" t="n">
+        <v>49556.0</v>
       </c>
       <c r="G82">
         <f t="shared" si="4"/>
         <v>146</v>
       </c>
-      <c r="H82">
-        <v>0</v>
+      <c r="H82" t="n">
+        <v>0.0</v>
       </c>
       <c r="I82">
         <f t="shared" si="3"/>
@@ -4200,15 +4201,15 @@
       <c r="D83" t="s">
         <v>159</v>
       </c>
-      <c r="F83">
-        <v>48411</v>
+      <c r="F83" t="n">
+        <v>48411.0</v>
       </c>
       <c r="G83">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="H83">
-        <v>0</v>
+      <c r="H83" t="n">
+        <v>0.0</v>
       </c>
       <c r="I83">
         <f t="shared" si="3"/>
@@ -4232,15 +4233,15 @@
       <c r="D84" t="s">
         <v>161</v>
       </c>
-      <c r="F84">
-        <v>49092</v>
+      <c r="F84" t="n">
+        <v>49092.0</v>
       </c>
       <c r="G84">
         <f t="shared" si="4"/>
         <v>152</v>
       </c>
-      <c r="H84">
-        <v>0</v>
+      <c r="H84" t="n">
+        <v>1.0</v>
       </c>
       <c r="I84">
         <f t="shared" si="3"/>
@@ -4264,15 +4265,15 @@
       <c r="D85" t="s">
         <v>163</v>
       </c>
-      <c r="F85">
-        <v>48201</v>
+      <c r="F85" t="n">
+        <v>48201.0</v>
       </c>
       <c r="G85">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="H85">
-        <v>1</v>
+      <c r="H85" t="n">
+        <v>0.0</v>
       </c>
       <c r="I85">
         <f t="shared" si="3"/>
@@ -4296,15 +4297,15 @@
       <c r="D86" t="s">
         <v>165</v>
       </c>
-      <c r="F86">
-        <v>48264</v>
+      <c r="F86" t="n">
+        <v>48264.0</v>
       </c>
       <c r="G86">
         <f t="shared" si="4"/>
         <v>102</v>
       </c>
-      <c r="H86">
-        <v>1</v>
+      <c r="H86" t="n">
+        <v>1.0</v>
       </c>
       <c r="I86">
         <f t="shared" si="3"/>
@@ -4328,15 +4329,15 @@
       <c r="D87" t="s">
         <v>167</v>
       </c>
-      <c r="F87">
-        <v>48805</v>
+      <c r="F87" t="n">
+        <v>48805.0</v>
       </c>
       <c r="G87">
         <f t="shared" si="4"/>
         <v>124</v>
       </c>
-      <c r="H87">
-        <v>0</v>
+      <c r="H87" t="n">
+        <v>3.0</v>
       </c>
       <c r="I87">
         <f t="shared" si="3"/>
@@ -4360,15 +4361,15 @@
       <c r="D88" t="s">
         <v>168</v>
       </c>
-      <c r="F88">
-        <v>48784</v>
+      <c r="F88" t="n">
+        <v>48784.0</v>
       </c>
       <c r="G88">
         <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="H88">
-        <v>0</v>
+      <c r="H88" t="n">
+        <v>1.0</v>
       </c>
       <c r="I88">
         <f t="shared" si="3"/>
@@ -4392,15 +4393,15 @@
       <c r="D89" t="s">
         <v>170</v>
       </c>
-      <c r="F89">
-        <v>47998</v>
+      <c r="F89" t="n">
+        <v>47998.0</v>
       </c>
       <c r="G89">
         <f t="shared" si="4"/>
         <v>116</v>
       </c>
-      <c r="H89">
-        <v>0</v>
+      <c r="H89" t="n">
+        <v>1.0</v>
       </c>
       <c r="I89">
         <f t="shared" si="3"/>
@@ -4424,15 +4425,15 @@
       <c r="D90" t="s">
         <v>172</v>
       </c>
-      <c r="F90">
-        <v>48278</v>
+      <c r="F90" t="n">
+        <v>48278.0</v>
       </c>
       <c r="G90">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="H90">
-        <v>0</v>
+      <c r="H90" t="n">
+        <v>0.0</v>
       </c>
       <c r="I90">
         <f t="shared" si="3"/>
@@ -4456,15 +4457,15 @@
       <c r="D91" t="s">
         <v>174</v>
       </c>
-      <c r="F91">
-        <v>47758</v>
+      <c r="F91" t="n">
+        <v>47758.0</v>
       </c>
       <c r="G91">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="H91">
-        <v>0</v>
+      <c r="H91" t="n">
+        <v>0.0</v>
       </c>
       <c r="I91">
         <f t="shared" si="3"/>
@@ -4488,15 +4489,15 @@
       <c r="D92" t="s">
         <v>176</v>
       </c>
-      <c r="F92">
-        <v>47156</v>
+      <c r="F92" t="n">
+        <v>47156.0</v>
       </c>
       <c r="G92">
         <f t="shared" si="4"/>
         <v>882</v>
       </c>
-      <c r="H92">
-        <v>0</v>
+      <c r="H92" t="n">
+        <v>0.0</v>
       </c>
       <c r="I92">
         <f t="shared" si="3"/>
@@ -4520,15 +4521,15 @@
       <c r="D93" t="s">
         <v>178</v>
       </c>
-      <c r="F93">
-        <v>48369</v>
+      <c r="F93" t="n">
+        <v>48369.0</v>
       </c>
       <c r="G93">
         <f t="shared" si="4"/>
         <v>870</v>
       </c>
-      <c r="H93">
-        <v>0</v>
+      <c r="H93" t="n">
+        <v>0.0</v>
       </c>
       <c r="I93">
         <f t="shared" si="3"/>
@@ -4552,15 +4553,15 @@
       <c r="D94" t="s">
         <v>180</v>
       </c>
-      <c r="F94">
-        <v>48040</v>
+      <c r="F94" t="n">
+        <v>48040.0</v>
       </c>
       <c r="G94">
         <f t="shared" si="4"/>
         <v>860</v>
       </c>
-      <c r="H94">
-        <v>0</v>
+      <c r="H94" t="n">
+        <v>0.0</v>
       </c>
       <c r="I94">
         <f t="shared" si="3"/>
@@ -4584,15 +4585,15 @@
       <c r="D95" t="s">
         <v>182</v>
       </c>
-      <c r="F95">
-        <v>49556</v>
+      <c r="F95" t="n">
+        <v>49556.0</v>
       </c>
       <c r="G95">
         <f t="shared" si="4"/>
         <v>920</v>
       </c>
-      <c r="H95">
-        <v>0</v>
+      <c r="H95" t="n">
+        <v>0.0</v>
       </c>
       <c r="I95">
         <f t="shared" si="3"/>
@@ -4616,15 +4617,15 @@
       <c r="D96" t="s">
         <v>184</v>
       </c>
-      <c r="F96">
-        <v>49225</v>
+      <c r="F96" t="n">
+        <v>49225.0</v>
       </c>
       <c r="G96">
         <f t="shared" si="4"/>
         <v>850</v>
       </c>
-      <c r="H96">
-        <v>0</v>
+      <c r="H96" t="n">
+        <v>0.0</v>
       </c>
       <c r="I96">
         <f t="shared" si="3"/>
@@ -4648,15 +4649,15 @@
       <c r="D97" t="s">
         <v>186</v>
       </c>
-      <c r="F97">
-        <v>48847</v>
+      <c r="F97" t="n">
+        <v>48847.0</v>
       </c>
       <c r="G97">
         <f t="shared" si="4"/>
         <v>920</v>
       </c>
-      <c r="H97">
-        <v>0</v>
+      <c r="H97" t="n">
+        <v>1.0</v>
       </c>
       <c r="I97">
         <f t="shared" si="3"/>
@@ -4680,15 +4681,15 @@
       <c r="D98" t="s">
         <v>189</v>
       </c>
-      <c r="F98">
-        <v>48840</v>
+      <c r="F98" t="n">
+        <v>48840.0</v>
       </c>
       <c r="G98">
         <f t="shared" si="4"/>
         <v>920</v>
       </c>
-      <c r="H98">
-        <v>0</v>
+      <c r="H98" t="n">
+        <v>0.0</v>
       </c>
       <c r="I98">
         <f t="shared" si="3"/>
@@ -4712,15 +4713,15 @@
       <c r="D99" t="s">
         <v>191</v>
       </c>
-      <c r="F99">
-        <v>48987</v>
+      <c r="F99" t="n">
+        <v>48987.0</v>
       </c>
       <c r="G99">
         <f t="shared" si="4"/>
         <v>876</v>
       </c>
-      <c r="H99">
-        <v>0</v>
+      <c r="H99" t="n">
+        <v>0.0</v>
       </c>
       <c r="I99">
         <f t="shared" si="3"/>
@@ -4744,15 +4745,15 @@
       <c r="D100" t="s">
         <v>193</v>
       </c>
-      <c r="F100">
-        <v>47998</v>
+      <c r="F100" t="n">
+        <v>47998.0</v>
       </c>
       <c r="G100">
         <f t="shared" si="4"/>
         <v>870</v>
       </c>
-      <c r="H100">
-        <v>1</v>
+      <c r="H100" t="n">
+        <v>1.0</v>
       </c>
       <c r="I100">
         <f t="shared" si="3"/>
@@ -4776,15 +4777,15 @@
       <c r="D101" t="s">
         <v>195</v>
       </c>
-      <c r="F101">
-        <v>48320</v>
+      <c r="F101" t="n">
+        <v>48320.0</v>
       </c>
       <c r="G101">
         <f t="shared" si="4"/>
         <v>846</v>
       </c>
-      <c r="H101">
-        <v>0</v>
+      <c r="H101" t="n">
+        <v>0.0</v>
       </c>
       <c r="I101">
         <f t="shared" si="3"/>
@@ -4808,15 +4809,15 @@
       <c r="D102" t="s">
         <v>197</v>
       </c>
-      <c r="F102">
-        <v>57808</v>
+      <c r="F102" t="n">
+        <v>57808.0</v>
       </c>
       <c r="G102">
         <f t="shared" si="4"/>
         <v>76</v>
       </c>
-      <c r="H102">
-        <v>0</v>
+      <c r="H102" t="n">
+        <v>0.0</v>
       </c>
       <c r="I102">
         <f t="shared" si="3"/>
@@ -4840,15 +4841,15 @@
       <c r="D103" t="s">
         <v>199</v>
       </c>
-      <c r="F103">
-        <v>57997</v>
+      <c r="F103" t="n">
+        <v>57997.0</v>
       </c>
       <c r="G103">
         <f t="shared" si="4"/>
         <v>176</v>
       </c>
-      <c r="H103">
-        <v>1</v>
+      <c r="H103" t="n">
+        <v>0.0</v>
       </c>
       <c r="I103">
         <f t="shared" si="3"/>
@@ -4872,15 +4873,15 @@
       <c r="D104" t="s">
         <v>201</v>
       </c>
-      <c r="F104">
-        <v>58046</v>
+      <c r="F104" t="n">
+        <v>58046.0</v>
       </c>
       <c r="G104">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="H104">
-        <v>0</v>
+      <c r="H104" t="n">
+        <v>1.0</v>
       </c>
       <c r="I104">
         <f t="shared" si="3"/>
@@ -4904,15 +4905,15 @@
       <c r="D105" t="s">
         <v>203</v>
       </c>
-      <c r="F105">
-        <v>58559</v>
+      <c r="F105" t="n">
+        <v>58559.0</v>
       </c>
       <c r="G105">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="H105">
-        <v>0</v>
+      <c r="H105" t="n">
+        <v>0.0</v>
       </c>
       <c r="I105">
         <f t="shared" si="3"/>
@@ -4936,15 +4937,15 @@
       <c r="D106" t="s">
         <v>205</v>
       </c>
-      <c r="F106">
-        <v>58384</v>
+      <c r="F106" t="n">
+        <v>58384.0</v>
       </c>
       <c r="G106">
         <f t="shared" si="4"/>
         <v>168</v>
       </c>
-      <c r="H106">
-        <v>0</v>
+      <c r="H106" t="n">
+        <v>0.0</v>
       </c>
       <c r="I106">
         <f t="shared" si="3"/>
@@ -4968,15 +4969,15 @@
       <c r="D107" t="s">
         <v>207</v>
       </c>
-      <c r="F107">
-        <v>57773</v>
+      <c r="F107" t="n">
+        <v>57773.0</v>
       </c>
       <c r="G107">
         <f t="shared" si="4"/>
         <v>108</v>
       </c>
-      <c r="H107">
-        <v>0</v>
+      <c r="H107" t="n">
+        <v>1.0</v>
       </c>
       <c r="I107">
         <f t="shared" si="3"/>
@@ -5000,15 +5001,15 @@
       <c r="D108" t="s">
         <v>210</v>
       </c>
-      <c r="F108">
-        <v>57724</v>
+      <c r="F108" t="n">
+        <v>57724.0</v>
       </c>
       <c r="G108">
         <f t="shared" si="4"/>
         <v>124</v>
       </c>
-      <c r="H108">
-        <v>0</v>
+      <c r="H108" t="n">
+        <v>0.0</v>
       </c>
       <c r="I108">
         <f t="shared" si="3"/>
@@ -5032,15 +5033,15 @@
       <c r="D109" t="s">
         <v>212</v>
       </c>
-      <c r="F109">
-        <v>58370</v>
+      <c r="F109" t="n">
+        <v>58370.0</v>
       </c>
       <c r="G109">
         <f t="shared" si="4"/>
         <v>108</v>
       </c>
-      <c r="H109">
-        <v>0</v>
+      <c r="H109" t="n">
+        <v>0.0</v>
       </c>
       <c r="I109">
         <f t="shared" si="3"/>
@@ -5064,15 +5065,15 @@
       <c r="D110" t="s">
         <v>214</v>
       </c>
-      <c r="F110">
-        <v>58067</v>
+      <c r="F110" t="n">
+        <v>58067.0</v>
       </c>
       <c r="G110">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="H110">
-        <v>0</v>
+      <c r="H110" t="n">
+        <v>0.0</v>
       </c>
       <c r="I110">
         <f t="shared" si="3"/>
@@ -5096,15 +5097,15 @@
       <c r="D111" t="s">
         <v>216</v>
       </c>
-      <c r="F111">
-        <v>58573</v>
+      <c r="F111" t="n">
+        <v>58573.0</v>
       </c>
       <c r="G111">
         <f t="shared" si="4"/>
         <v>188</v>
       </c>
-      <c r="H111">
-        <v>0</v>
+      <c r="H111" t="n">
+        <v>0.0</v>
       </c>
       <c r="I111">
         <f t="shared" si="3"/>
@@ -5128,15 +5129,15 @@
       <c r="D112" t="s">
         <v>218</v>
       </c>
-      <c r="F112">
-        <v>58580</v>
+      <c r="F112" t="n">
+        <v>58580.0</v>
       </c>
       <c r="G112">
         <f t="shared" si="4"/>
         <v>1054</v>
       </c>
-      <c r="H112">
-        <v>1</v>
+      <c r="H112" t="n">
+        <v>1.0</v>
       </c>
       <c r="I112">
         <f t="shared" si="3"/>
@@ -5160,15 +5161,15 @@
       <c r="D113" t="s">
         <v>220</v>
       </c>
-      <c r="F113">
-        <v>58384</v>
+      <c r="F113" t="n">
+        <v>58384.0</v>
       </c>
       <c r="G113">
         <f t="shared" si="4"/>
         <v>922</v>
       </c>
-      <c r="H113">
-        <v>0</v>
+      <c r="H113" t="n">
+        <v>0.0</v>
       </c>
       <c r="I113">
         <f t="shared" si="3"/>
@@ -5192,15 +5193,15 @@
       <c r="D114" t="s">
         <v>222</v>
       </c>
-      <c r="F114">
-        <v>57864</v>
+      <c r="F114" t="n">
+        <v>57864.0</v>
       </c>
       <c r="G114">
         <f t="shared" si="4"/>
         <v>1096</v>
       </c>
-      <c r="H114">
-        <v>0</v>
+      <c r="H114" t="n">
+        <v>0.0</v>
       </c>
       <c r="I114">
         <f t="shared" si="3"/>
@@ -5224,15 +5225,15 @@
       <c r="D115" t="s">
         <v>224</v>
       </c>
-      <c r="F115">
-        <v>57766</v>
+      <c r="F115" t="n">
+        <v>57766.0</v>
       </c>
       <c r="G115">
         <f t="shared" si="4"/>
         <v>1048</v>
       </c>
-      <c r="H115">
-        <v>0</v>
+      <c r="H115" t="n">
+        <v>0.0</v>
       </c>
       <c r="I115">
         <f t="shared" si="3"/>
@@ -5256,15 +5257,15 @@
       <c r="D116" t="s">
         <v>226</v>
       </c>
-      <c r="F116">
-        <v>58060</v>
+      <c r="F116" t="n">
+        <v>58060.0</v>
       </c>
       <c r="G116">
         <f t="shared" si="4"/>
         <v>1092</v>
       </c>
-      <c r="H116">
-        <v>1</v>
+      <c r="H116" t="n">
+        <v>0.0</v>
       </c>
       <c r="I116">
         <f t="shared" si="3"/>
@@ -5288,15 +5289,15 @@
       <c r="D117" t="s">
         <v>228</v>
       </c>
-      <c r="F117">
-        <v>58144</v>
+      <c r="F117" t="n">
+        <v>58144.0</v>
       </c>
       <c r="G117">
         <f t="shared" si="4"/>
         <v>1060</v>
       </c>
-      <c r="H117">
-        <v>1</v>
+      <c r="H117" t="n">
+        <v>0.0</v>
       </c>
       <c r="I117">
         <f t="shared" si="3"/>
@@ -5320,15 +5321,15 @@
       <c r="D118" t="s">
         <v>230</v>
       </c>
-      <c r="F118">
-        <v>57647</v>
+      <c r="F118" t="n">
+        <v>57647.0</v>
       </c>
       <c r="G118">
         <f t="shared" si="4"/>
         <v>1090</v>
       </c>
-      <c r="H118">
-        <v>0</v>
+      <c r="H118" t="n">
+        <v>0.0</v>
       </c>
       <c r="I118">
         <f t="shared" si="3"/>
@@ -5352,15 +5353,15 @@
       <c r="D119" t="s">
         <v>232</v>
       </c>
-      <c r="F119">
-        <v>58053</v>
+      <c r="F119" t="n">
+        <v>58053.0</v>
       </c>
       <c r="G119">
         <f t="shared" si="4"/>
         <v>1030</v>
       </c>
-      <c r="H119">
-        <v>0</v>
+      <c r="H119" t="n">
+        <v>1.0</v>
       </c>
       <c r="I119">
         <f t="shared" si="3"/>
@@ -5384,15 +5385,15 @@
       <c r="D120" t="s">
         <v>234</v>
       </c>
-      <c r="F120">
-        <v>58776</v>
+      <c r="F120" t="n">
+        <v>58776.0</v>
       </c>
       <c r="G120">
         <f t="shared" si="4"/>
         <v>1020</v>
       </c>
-      <c r="H120">
-        <v>1</v>
+      <c r="H120" t="n">
+        <v>0.0</v>
       </c>
       <c r="I120">
         <f t="shared" si="3"/>
@@ -5416,15 +5417,15 @@
       <c r="D121" t="s">
         <v>236</v>
       </c>
-      <c r="F121">
-        <v>57183</v>
+      <c r="F121" t="n">
+        <v>57183.0</v>
       </c>
       <c r="G121">
         <f t="shared" si="4"/>
         <v>920</v>
       </c>
-      <c r="H121">
-        <v>0</v>
+      <c r="H121" t="n">
+        <v>0.0</v>
       </c>
       <c r="I121">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
excel with updated graphics
</commit_message>
<xml_diff>
--- a/results-assignment.xlsx
+++ b/results-assignment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="results-assignment" sheetId="1" r:id="rId1"/>
@@ -2204,7 +2204,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2563,11 +2562,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="650281456"/>
-        <c:axId val="650281848"/>
+        <c:axId val="155917000"/>
+        <c:axId val="155917392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="650281456"/>
+        <c:axId val="155917000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,7 +2608,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650281848"/>
+        <c:crossAx val="155917392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2617,7 +2616,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="650281848"/>
+        <c:axId val="155917392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2668,7 +2667,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650281456"/>
+        <c:crossAx val="155917000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2682,7 +2681,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2794,7 +2792,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3153,11 +3150,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="650292040"/>
-        <c:axId val="650292432"/>
+        <c:axId val="199679128"/>
+        <c:axId val="199686184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="650292040"/>
+        <c:axId val="199679128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +3196,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650292432"/>
+        <c:crossAx val="199686184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3207,7 +3204,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="650292432"/>
+        <c:axId val="199686184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3258,7 +3255,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650292040"/>
+        <c:crossAx val="199679128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3272,7 +3269,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3384,7 +3380,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3743,11 +3738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="721851824"/>
-        <c:axId val="721857704"/>
+        <c:axId val="199681872"/>
+        <c:axId val="199685792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="721851824"/>
+        <c:axId val="199681872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,7 +3784,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721857704"/>
+        <c:crossAx val="199685792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3797,7 +3792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="721857704"/>
+        <c:axId val="199685792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3848,7 +3843,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721851824"/>
+        <c:crossAx val="199681872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3862,7 +3857,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3974,7 +3968,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4333,11 +4326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="934253464"/>
-        <c:axId val="934253856"/>
+        <c:axId val="199683440"/>
+        <c:axId val="199679912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="934253464"/>
+        <c:axId val="199683440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4379,7 +4372,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="934253856"/>
+        <c:crossAx val="199679912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4387,7 +4380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="934253856"/>
+        <c:axId val="199679912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4438,7 +4431,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="934253464"/>
+        <c:crossAx val="199683440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4452,7 +4445,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4923,11 +4915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="662812704"/>
-        <c:axId val="662813096"/>
+        <c:axId val="199681088"/>
+        <c:axId val="199683832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="662812704"/>
+        <c:axId val="199681088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4969,7 +4961,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662813096"/>
+        <c:crossAx val="199683832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4977,7 +4969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="662813096"/>
+        <c:axId val="199683832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,7 +5020,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="662812704"/>
+        <c:crossAx val="199681088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5154,7 +5146,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5523,11 +5514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="721860056"/>
-        <c:axId val="721860448"/>
+        <c:axId val="199685008"/>
+        <c:axId val="199682656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="721860056"/>
+        <c:axId val="199685008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5569,7 +5560,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721860448"/>
+        <c:crossAx val="199682656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5577,7 +5568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="721860448"/>
+        <c:axId val="199682656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5628,7 +5619,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721860056"/>
+        <c:crossAx val="199685008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5642,7 +5633,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9505,8 +9495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9586,19 +9576,19 @@
         <v>96997</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G66" si="0">F2-B2</f>
+        <f>F2-B2</f>
         <v>26</v>
       </c>
       <c r="H2">
         <v>19</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I65" si="1">(F2-B2)/B2</f>
+        <f>(F2-B2)/B2</f>
         <v>2.6812139711872621E-4</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J66" si="2">F2*100/B2</f>
-        <v>100.02681213971188</v>
+        <f>(F2*100/B2)-100</f>
+        <v>2.6812139711879013E-2</v>
       </c>
       <c r="L2">
         <v>84</v>
@@ -9639,19 +9629,19 @@
         <v>97081</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
+        <f>F3-B3</f>
         <v>-46</v>
       </c>
       <c r="H3">
         <v>26</v>
       </c>
       <c r="I3">
-        <f t="shared" si="1"/>
+        <f>(F3-B3)/B3</f>
         <v>-4.7360672109712028E-4</v>
       </c>
       <c r="J3">
-        <f t="shared" si="2"/>
-        <v>99.952639327890282</v>
+        <f t="shared" ref="J3:J66" si="0">(F3*100/B3)-100</f>
+        <v>-4.7360672109718394E-2</v>
       </c>
       <c r="L3">
         <v>84</v>
@@ -9692,19 +9682,19 @@
         <v>98394</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>F4-B4</f>
         <v>-30</v>
       </c>
       <c r="H4">
         <v>7</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f>(F4-B4)/B4</f>
         <v>-3.0480370641307E-4</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
-        <v>99.969519629358686</v>
+        <f t="shared" si="0"/>
+        <v>-3.0480370641313925E-2</v>
       </c>
       <c r="L4">
         <v>86</v>
@@ -9745,19 +9735,19 @@
         <v>97123</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f>F5-B5</f>
         <v>-160</v>
       </c>
       <c r="H5">
         <v>9</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f>(F5-B5)/B5</f>
         <v>-1.6446861219329173E-3</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>99.835531387806711</v>
+        <f t="shared" si="0"/>
+        <v>-0.16446861219328923</v>
       </c>
       <c r="L5">
         <v>84</v>
@@ -9798,19 +9788,19 @@
         <v>95791</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6-B6</f>
         <v>128</v>
       </c>
       <c r="H6">
         <v>6</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f>(F6-B6)/B6</f>
         <v>1.3380303774709135E-3</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>100.13380303774709</v>
+        <f t="shared" si="0"/>
+        <v>0.1338030377470858</v>
       </c>
       <c r="L6">
         <v>83</v>
@@ -9851,19 +9841,19 @@
         <v>94261</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7-B7</f>
         <v>98</v>
       </c>
       <c r="H7">
         <v>7</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f>(F7-B7)/B7</f>
         <v>1.0407484893217081E-3</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>100.10407484893217</v>
+        <f t="shared" si="0"/>
+        <v>0.10407484893217145</v>
       </c>
       <c r="L7">
         <v>81</v>
@@ -9904,19 +9894,19 @@
         <v>97972</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f>F8-B8</f>
         <v>38</v>
       </c>
       <c r="H8">
         <v>5</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f>(F8-B8)/B8</f>
         <v>3.8801641922110811E-4</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
-        <v>100.03880164192211</v>
+        <f t="shared" si="0"/>
+        <v>3.8801641922106E-2</v>
       </c>
       <c r="L8">
         <v>85</v>
@@ -9957,19 +9947,19 @@
         <v>97937</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f>F9-B9</f>
         <v>14</v>
       </c>
       <c r="H9">
         <v>5</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f>(F9-B9)/B9</f>
         <v>1.429694760168704E-4</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
-        <v>100.01429694760169</v>
+        <f t="shared" si="0"/>
+        <v>1.4296947601692978E-2</v>
       </c>
       <c r="L9">
         <v>85</v>
@@ -10010,19 +10000,19 @@
         <v>96591</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f>F10-B10</f>
         <v>76</v>
       </c>
       <c r="H10">
         <v>6</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f>(F10-B10)/B10</f>
         <v>7.8744236647153288E-4</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
-        <v>100.07874423664715</v>
+        <f t="shared" si="0"/>
+        <v>7.8744236647153798E-2</v>
       </c>
       <c r="L10">
         <v>84</v>
@@ -10063,19 +10053,19 @@
         <v>97881</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f>F11-B11</f>
         <v>-26</v>
       </c>
       <c r="H11">
         <v>15</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f>(F11-B11)/B11</f>
         <v>-2.6555813169640578E-4</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
-        <v>99.973444186830363</v>
+        <f t="shared" si="0"/>
+        <v>-2.6555813169636622E-2</v>
       </c>
       <c r="L11">
         <v>85</v>
@@ -10116,19 +10106,19 @@
         <v>95016</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f>F12-B12</f>
         <v>-110</v>
       </c>
       <c r="H12">
         <v>4</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f>(F12-B12)/B12</f>
         <v>-1.156361036940479E-3</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
-        <v>99.884363896305956</v>
+        <f t="shared" si="0"/>
+        <v>-0.11563610369404387</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -10169,19 +10159,19 @@
         <v>95254</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f>F13-B13</f>
         <v>-420</v>
       </c>
       <c r="H13">
         <v>5</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f>(F13-B13)/B13</f>
         <v>-4.3899073938583107E-3</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
-        <v>99.561009260614171</v>
+        <f t="shared" si="0"/>
+        <v>-0.43899073938582944</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -10222,19 +10212,19 @@
         <v>95331</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>F14-B14</f>
         <v>-300</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f>(F14-B14)/B14</f>
         <v>-3.1370580669448193E-3</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
-        <v>99.686294193305514</v>
+        <f t="shared" si="0"/>
+        <v>-0.313705806694486</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -10275,19 +10265,19 @@
         <v>95471</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f>F15-B15</f>
         <v>-180</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f>(F15-B15)/B15</f>
         <v>-1.8818412771429468E-3</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
-        <v>99.811815872285706</v>
+        <f t="shared" si="0"/>
+        <v>-0.18818412771429394</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -10328,19 +10318,19 @@
         <v>94890</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f>F16-B16</f>
         <v>-80</v>
       </c>
       <c r="H16">
         <v>4</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f>(F16-B16)/B16</f>
         <v>-8.4237127513951779E-4</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
-        <v>99.915762872486042</v>
+        <f t="shared" si="0"/>
+        <v>-8.4237127513958399E-2</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -10381,19 +10371,19 @@
         <v>95983</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f>F17-B17</f>
         <v>-300</v>
       </c>
       <c r="H17">
         <v>5</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f>(F17-B17)/B17</f>
         <v>-3.1158148375102562E-3</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
-        <v>99.688418516248973</v>
+        <f t="shared" si="0"/>
+        <v>-0.31158148375102712</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -10434,19 +10424,19 @@
         <v>95177</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f>F18-B18</f>
         <v>-66</v>
       </c>
       <c r="H18">
         <v>3</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f>(F18-B18)/B18</f>
         <v>-6.9296431233791455E-4</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
-        <v>99.930703568766205</v>
+        <f t="shared" si="0"/>
+        <v>-6.929643123379492E-2</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -10487,19 +10477,19 @@
         <v>94701</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f>F19-B19</f>
         <v>-60</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f>(F19-B19)/B19</f>
         <v>-6.3317187450533444E-4</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
-        <v>99.936682812549464</v>
+        <f t="shared" si="0"/>
+        <v>-6.3317187450536494E-2</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -10540,19 +10530,19 @@
         <v>94035</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f>F20-B20</f>
         <v>-192</v>
       </c>
       <c r="H20">
         <v>5</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f>(F20-B20)/B20</f>
         <v>-2.0376325257091916E-3</v>
       </c>
       <c r="J20">
-        <f t="shared" si="2"/>
-        <v>99.796236747429077</v>
+        <f t="shared" si="0"/>
+        <v>-0.20376325257092276</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -10593,19 +10583,19 @@
         <v>95317</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f>F21-B21</f>
         <v>-300</v>
       </c>
       <c r="H21">
         <v>6</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f>(F21-B21)/B21</f>
         <v>-3.1375173870755199E-3</v>
       </c>
       <c r="J21">
-        <f t="shared" si="2"/>
-        <v>99.686248261292448</v>
+        <f t="shared" si="0"/>
+        <v>-0.31375173870755191</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -10646,19 +10636,19 @@
         <v>117356</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f>F22-B22</f>
         <v>-4</v>
       </c>
       <c r="H22">
         <v>7</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
+        <f>(F22-B22)/B22</f>
         <v>-3.4083162917518748E-5</v>
       </c>
       <c r="J22">
-        <f t="shared" si="2"/>
-        <v>99.996591683708246</v>
+        <f t="shared" si="0"/>
+        <v>-3.4083162917539767E-3</v>
       </c>
       <c r="L22">
         <v>110</v>
@@ -10699,19 +10689,19 @@
         <v>116183</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
+        <f>F23-B23</f>
         <v>-70</v>
       </c>
       <c r="H23">
         <v>6</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f>(F23-B23)/B23</f>
         <v>-6.0213499866670103E-4</v>
       </c>
       <c r="J23">
-        <f t="shared" si="2"/>
-        <v>99.939786500133323</v>
+        <f t="shared" si="0"/>
+        <v>-6.0213499866677012E-2</v>
       </c>
       <c r="L23">
         <v>108</v>
@@ -10752,19 +10742,19 @@
         <v>115397</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f>F24-B24</f>
         <v>94</v>
       </c>
       <c r="H24">
         <v>5</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f>(F24-B24)/B24</f>
         <v>8.1524331543845346E-4</v>
       </c>
       <c r="J24">
-        <f t="shared" si="2"/>
-        <v>100.08152433154385</v>
+        <f t="shared" si="0"/>
+        <v>8.1524331543846529E-2</v>
       </c>
       <c r="L24">
         <v>107</v>
@@ -10805,19 +10795,19 @@
         <v>116302</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f>F25-B25</f>
         <v>34</v>
       </c>
       <c r="H25">
         <v>12</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f>(F25-B25)/B25</f>
         <v>2.9242783913028522E-4</v>
       </c>
       <c r="J25">
-        <f t="shared" si="2"/>
-        <v>100.02924278391303</v>
+        <f t="shared" si="0"/>
+        <v>2.9242783913034032E-2</v>
       </c>
       <c r="L25">
         <v>108</v>
@@ -10858,19 +10848,19 @@
         <v>116745</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f>F26-B26</f>
         <v>66</v>
       </c>
       <c r="H26">
         <v>14</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f>(F26-B26)/B26</f>
         <v>5.6565448795413051E-4</v>
       </c>
       <c r="J26">
-        <f t="shared" si="2"/>
-        <v>100.05656544879541</v>
+        <f t="shared" si="0"/>
+        <v>5.6565448795410589E-2</v>
       </c>
       <c r="L26">
         <v>109</v>
@@ -10911,19 +10901,19 @@
         <v>116022</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f>F27-B27</f>
         <v>-1066</v>
       </c>
       <c r="H27">
         <v>14</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
+        <f>(F27-B27)/B27</f>
         <v>-9.1042634599617384E-3</v>
       </c>
       <c r="J27">
-        <f t="shared" si="2"/>
-        <v>99.089573654003829</v>
+        <f t="shared" si="0"/>
+        <v>-0.91042634599617145</v>
       </c>
       <c r="L27">
         <v>108</v>
@@ -10964,19 +10954,19 @@
         <v>116358</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
+        <f>F28-B28</f>
         <v>-74</v>
       </c>
       <c r="H28">
         <v>14</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
+        <f>(F28-B28)/B28</f>
         <v>-6.3556410608767351E-4</v>
       </c>
       <c r="J28">
-        <f t="shared" si="2"/>
-        <v>99.936443589391232</v>
+        <f t="shared" si="0"/>
+        <v>-6.3556410608768488E-2</v>
       </c>
       <c r="L28">
         <v>108</v>
@@ -11017,19 +11007,19 @@
         <v>116113</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f>F29-B29</f>
         <v>30</v>
       </c>
       <c r="H29">
         <v>16</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
+        <f>(F29-B29)/B29</f>
         <v>2.5843577440279802E-4</v>
       </c>
       <c r="J29">
-        <f t="shared" si="2"/>
-        <v>100.02584357744028</v>
+        <f t="shared" si="0"/>
+        <v>2.5843577440284093E-2</v>
       </c>
       <c r="L29">
         <v>108</v>
@@ -11070,19 +11060,19 @@
         <v>116043</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f>F30-B30</f>
         <v>-118</v>
       </c>
       <c r="H30">
         <v>5</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f>(F30-B30)/B30</f>
         <v>-1.0158314752799994E-3</v>
       </c>
       <c r="J30">
-        <f t="shared" si="2"/>
-        <v>99.898416852471996</v>
+        <f t="shared" si="0"/>
+        <v>-0.10158314752800379</v>
       </c>
       <c r="L30">
         <v>108</v>
@@ -11123,19 +11113,19 @@
         <v>115334</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f>F31-B31</f>
         <v>90</v>
       </c>
       <c r="H31">
         <v>5</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f>(F31-B31)/B31</f>
         <v>7.8095171982923192E-4</v>
       </c>
       <c r="J31">
-        <f t="shared" si="2"/>
-        <v>100.07809517198292</v>
+        <f t="shared" si="0"/>
+        <v>7.8095171982923262E-2</v>
       </c>
       <c r="L31">
         <v>107</v>
@@ -11176,19 +11166,19 @@
         <v>113988</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
+        <f>F32-B32</f>
         <v>-9078</v>
       </c>
       <c r="H32">
         <v>5</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
+        <f>(F32-B32)/B32</f>
         <v>-7.3765296670079472E-2</v>
       </c>
       <c r="J32">
-        <f t="shared" si="2"/>
-        <v>92.623470332992056</v>
+        <f t="shared" si="0"/>
+        <v>-7.3765296670079437</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -11229,19 +11219,19 @@
         <v>113449</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
+        <f>F33-B33</f>
         <v>-9286</v>
       </c>
       <c r="H33">
         <v>4</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
+        <f>(F33-B33)/B33</f>
         <v>-7.5658939992667124E-2</v>
       </c>
       <c r="J33">
-        <f t="shared" si="2"/>
-        <v>92.434106000733294</v>
+        <f t="shared" si="0"/>
+        <v>-7.5658939992667058</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -11282,19 +11272,19 @@
         <v>113855</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <f>F34-B34</f>
         <v>-4356</v>
       </c>
       <c r="H34">
         <v>4</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f>(F34-B34)/B34</f>
         <v>-3.6849362580470515E-2</v>
       </c>
       <c r="J34">
-        <f t="shared" si="2"/>
-        <v>96.315063741952955</v>
+        <f t="shared" si="0"/>
+        <v>-3.6849362580470455</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -11335,19 +11325,19 @@
         <v>114752</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f>F35-B35</f>
         <v>-9800</v>
       </c>
       <c r="H35">
         <v>4</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f>(F35-B35)/B35</f>
         <v>-7.8681996274648336E-2</v>
       </c>
       <c r="J35">
-        <f t="shared" si="2"/>
-        <v>92.131800372535167</v>
+        <f t="shared" si="0"/>
+        <v>-7.8681996274648327</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -11388,19 +11378,19 @@
         <v>112503</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f>F36-B36</f>
         <v>-8974</v>
       </c>
       <c r="H36">
         <v>4</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
+        <f>(F36-B36)/B36</f>
         <v>-7.387406669575311E-2</v>
       </c>
       <c r="J36">
-        <f t="shared" si="2"/>
-        <v>92.612593330424687</v>
+        <f t="shared" si="0"/>
+        <v>-7.3874066695753129</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -11441,19 +11431,19 @@
         <v>113701</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f>F37-B37</f>
         <v>-8782</v>
       </c>
       <c r="H37">
         <v>4</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f>(F37-B37)/B37</f>
         <v>-7.1699746087212107E-2</v>
       </c>
       <c r="J37">
-        <f t="shared" si="2"/>
-        <v>92.830025391278795</v>
+        <f t="shared" si="0"/>
+        <v>-7.1699746087212048</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -11494,19 +11484,19 @@
         <v>114065</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f>F38-B38</f>
         <v>-7212</v>
       </c>
       <c r="H38">
         <v>4</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f>(F38-B38)/B38</f>
         <v>-5.9467170197151975E-2</v>
       </c>
       <c r="J38">
-        <f t="shared" si="2"/>
-        <v>94.053282980284806</v>
+        <f t="shared" si="0"/>
+        <v>-5.9467170197151944</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -11547,19 +11537,19 @@
         <v>114030</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f>F39-B39</f>
         <v>-862</v>
       </c>
       <c r="H39">
         <v>4</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
+        <f>(F39-B39)/B39</f>
         <v>-7.5026981861226194E-3</v>
       </c>
       <c r="J39">
-        <f t="shared" si="2"/>
-        <v>99.249730181387733</v>
+        <f t="shared" si="0"/>
+        <v>-0.75026981861226716</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -11600,19 +11590,19 @@
         <v>115074</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f>F40-B40</f>
         <v>-10250</v>
       </c>
       <c r="H40">
         <v>10</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
+        <f>(F40-B40)/B40</f>
         <v>-8.1788005489770513E-2</v>
       </c>
       <c r="J40">
-        <f t="shared" si="2"/>
-        <v>91.821199451022949</v>
+        <f t="shared" si="0"/>
+        <v>-8.1788005489770512</v>
       </c>
       <c r="L40">
         <v>0</v>
@@ -11653,19 +11643,19 @@
         <v>114184</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f>F41-B41</f>
         <v>-318</v>
       </c>
       <c r="H41">
         <v>12</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
+        <f>(F41-B41)/B41</f>
         <v>-2.777244065605841E-3</v>
       </c>
       <c r="J41">
-        <f t="shared" si="2"/>
-        <v>99.72227559343942</v>
+        <f t="shared" si="0"/>
+        <v>-0.27772440656057995</v>
       </c>
       <c r="L41">
         <v>0</v>
@@ -11706,19 +11696,19 @@
         <v>19896</v>
       </c>
       <c r="G42">
+        <f>F42-B42</f>
+        <v>22</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <f>(F42-B42)/B42</f>
+        <v>1.1069739357955116E-3</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="1"/>
-        <v>1.1069739357955116E-3</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="2"/>
-        <v>100.11069739357956</v>
+        <v>0.11069739357955655</v>
       </c>
       <c r="L42">
         <v>18</v>
@@ -11759,19 +11749,19 @@
         <v>19854</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f>F43-B43</f>
         <v>42</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
+        <f>(F43-B43)/B43</f>
         <v>2.1199273167777106E-3</v>
       </c>
       <c r="J43">
-        <f t="shared" si="2"/>
-        <v>100.21199273167777</v>
+        <f t="shared" si="0"/>
+        <v>0.21199273167776767</v>
       </c>
       <c r="L43">
         <v>18</v>
@@ -11812,19 +11802,19 @@
         <v>19931</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
+        <f>F44-B44</f>
         <v>58</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
+        <f>(F44-B44)/B44</f>
         <v>2.9185326825340915E-3</v>
       </c>
       <c r="J44">
-        <f t="shared" si="2"/>
-        <v>100.2918532682534</v>
+        <f t="shared" si="0"/>
+        <v>0.29185326825340496</v>
       </c>
       <c r="L44">
         <v>18</v>
@@ -11865,19 +11855,19 @@
         <v>19194</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
+        <f>F45-B45</f>
         <v>40</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
+        <f>(F45-B45)/B45</f>
         <v>2.0883366398663466E-3</v>
       </c>
       <c r="J45">
-        <f t="shared" si="2"/>
-        <v>100.20883366398664</v>
+        <f t="shared" si="0"/>
+        <v>0.20883366398663838</v>
       </c>
       <c r="L45">
         <v>17</v>
@@ -11918,19 +11908,19 @@
         <v>19495</v>
       </c>
       <c r="G46">
+        <f>F46-B46</f>
+        <v>44</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f>(F46-B46)/B46</f>
+        <v>2.2620944938563569E-3</v>
+      </c>
+      <c r="J46">
         <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="1"/>
-        <v>2.2620944938563569E-3</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="2"/>
-        <v>100.22620944938564</v>
+        <v>0.22620944938563525</v>
       </c>
       <c r="L46">
         <v>17</v>
@@ -11971,19 +11961,19 @@
         <v>19945</v>
       </c>
       <c r="G47">
+        <f>F47-B47</f>
+        <v>54</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f>(F47-B47)/B47</f>
+        <v>2.7147956362173846E-3</v>
+      </c>
+      <c r="J47">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="1"/>
-        <v>2.7147956362173846E-3</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="2"/>
-        <v>100.27147956362174</v>
+        <v>0.27147956362173886</v>
       </c>
       <c r="L47">
         <v>18</v>
@@ -12024,19 +12014,19 @@
         <v>19215</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
+        <f>F48-B48</f>
         <v>36</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
+        <f>(F48-B48)/B48</f>
         <v>1.8770530267480056E-3</v>
       </c>
       <c r="J48">
-        <f t="shared" si="2"/>
-        <v>100.1877053026748</v>
+        <f t="shared" si="0"/>
+        <v>0.18770530267480012</v>
       </c>
       <c r="L48">
         <v>17</v>
@@ -12077,19 +12067,19 @@
         <v>19390</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
+        <f>F49-B49</f>
         <v>40</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
+        <f>(F49-B49)/B49</f>
         <v>2.0671834625322996E-3</v>
       </c>
       <c r="J49">
-        <f t="shared" si="2"/>
-        <v>100.20671834625323</v>
+        <f t="shared" si="0"/>
+        <v>0.2067183462532256</v>
       </c>
       <c r="L49">
         <v>17</v>
@@ -12130,19 +12120,19 @@
         <v>19208</v>
       </c>
       <c r="G50">
+        <f>F50-B50</f>
+        <v>52</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f>(F50-B50)/B50</f>
+        <v>2.7145541866778031E-3</v>
+      </c>
+      <c r="J50">
         <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="1"/>
-        <v>2.7145541866778031E-3</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="2"/>
-        <v>100.27145541866778</v>
+        <v>0.27145541866778444</v>
       </c>
       <c r="L50">
         <v>17</v>
@@ -12183,19 +12173,19 @@
         <v>19833</v>
       </c>
       <c r="G51">
+        <f>F51-B51</f>
+        <v>52</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <f>(F51-B51)/B51</f>
+        <v>2.6287851979171933E-3</v>
+      </c>
+      <c r="J51">
         <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="1"/>
-        <v>2.6287851979171933E-3</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="2"/>
-        <v>100.26287851979171</v>
+        <v>0.26287851979171251</v>
       </c>
       <c r="L51">
         <v>18</v>
@@ -12236,19 +12226,19 @@
         <v>19144</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f>F52-B52</f>
         <v>100</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
-        <f t="shared" si="1"/>
+        <f>(F52-B52)/B52</f>
         <v>5.2509976895610162E-3</v>
       </c>
       <c r="J52">
-        <f t="shared" si="2"/>
-        <v>100.5250997689561</v>
+        <f t="shared" si="0"/>
+        <v>0.52509976895609611</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -12289,19 +12279,19 @@
         <v>19312</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f>F53-B53</f>
         <v>50</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53">
-        <f t="shared" si="1"/>
+        <f>(F53-B53)/B53</f>
         <v>2.5957844460595993E-3</v>
       </c>
       <c r="J53">
-        <f t="shared" si="2"/>
-        <v>100.25957844460596</v>
+        <f t="shared" si="0"/>
+        <v>0.25957844460596391</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -12342,19 +12332,19 @@
         <v>19711</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
+        <f>F54-B54</f>
         <v>0</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <f t="shared" si="1"/>
+        <f>(F54-B54)/B54</f>
         <v>0</v>
       </c>
       <c r="J54">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -12395,19 +12385,19 @@
         <v>18835</v>
       </c>
       <c r="G55">
+        <f>F55-B55</f>
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <f>(F55-B55)/B55</f>
+        <v>0</v>
+      </c>
+      <c r="J55">
         <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J55">
-        <f t="shared" si="2"/>
-        <v>100</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -12448,19 +12438,19 @@
         <v>19060</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
+        <f>F56-B56</f>
         <v>80</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56">
-        <f t="shared" si="1"/>
+        <f>(F56-B56)/B56</f>
         <v>4.2149631190727078E-3</v>
       </c>
       <c r="J56">
-        <f t="shared" si="2"/>
-        <v>100.42149631190728</v>
+        <f t="shared" si="0"/>
+        <v>0.42149631190727632</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -12501,19 +12491,19 @@
         <v>19214</v>
       </c>
       <c r="G57">
-        <f t="shared" si="0"/>
+        <f>F57-B57</f>
         <v>88</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
       <c r="I57">
-        <f t="shared" si="1"/>
+        <f>(F57-B57)/B57</f>
         <v>4.6010666108961627E-3</v>
       </c>
       <c r="J57">
-        <f t="shared" si="2"/>
-        <v>100.46010666108961</v>
+        <f t="shared" si="0"/>
+        <v>0.46010666108961118</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -12554,19 +12544,19 @@
         <v>19326</v>
       </c>
       <c r="G58">
-        <f t="shared" si="0"/>
+        <f>F58-B58</f>
         <v>50</v>
       </c>
       <c r="H58">
         <v>1</v>
       </c>
       <c r="I58">
-        <f t="shared" si="1"/>
+        <f>(F58-B58)/B58</f>
         <v>2.5938991492010792E-3</v>
       </c>
       <c r="J58">
-        <f t="shared" si="2"/>
-        <v>100.25938991492011</v>
+        <f t="shared" si="0"/>
+        <v>0.25938991492010643</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -12607,19 +12597,19 @@
         <v>19137</v>
       </c>
       <c r="G59">
-        <f t="shared" si="0"/>
+        <f>F59-B59</f>
         <v>84</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59">
-        <f t="shared" si="1"/>
+        <f>(F59-B59)/B59</f>
         <v>4.4087545268461656E-3</v>
       </c>
       <c r="J59">
-        <f t="shared" si="2"/>
-        <v>100.44087545268462</v>
+        <f t="shared" si="0"/>
+        <v>0.44087545268462236</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -12660,19 +12650,19 @@
         <v>19004</v>
       </c>
       <c r="G60">
-        <f t="shared" si="0"/>
+        <f>F60-B60</f>
         <v>84</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60">
-        <f t="shared" si="1"/>
+        <f>(F60-B60)/B60</f>
         <v>4.4397463002114161E-3</v>
       </c>
       <c r="J60">
-        <f t="shared" si="2"/>
-        <v>100.44397463002115</v>
+        <f t="shared" si="0"/>
+        <v>0.44397463002114534</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -12713,19 +12703,19 @@
         <v>18758</v>
       </c>
       <c r="G61">
-        <f t="shared" si="0"/>
+        <f>F61-B61</f>
         <v>0</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="I61">
-        <f t="shared" si="1"/>
+        <f>(F61-B61)/B61</f>
         <v>0</v>
       </c>
       <c r="J61">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -12766,19 +12756,19 @@
         <v>23257</v>
       </c>
       <c r="G62">
+        <f>F62-B62</f>
+        <v>98</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <f>(F62-B62)/B62</f>
+        <v>4.231616218316853E-3</v>
+      </c>
+      <c r="J62">
         <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <f t="shared" si="1"/>
-        <v>4.231616218316853E-3</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="2"/>
-        <v>100.42316162183168</v>
+        <v>0.4231616218316816</v>
       </c>
       <c r="L62">
         <v>22</v>
@@ -12819,19 +12809,19 @@
         <v>23390</v>
       </c>
       <c r="G63">
+        <f>F63-B63</f>
+        <v>92</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f>(F63-B63)/B63</f>
+        <v>3.9488368100266116E-3</v>
+      </c>
+      <c r="J63">
         <f t="shared" si="0"/>
-        <v>92</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="1"/>
-        <v>3.9488368100266116E-3</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="2"/>
-        <v>100.39488368100267</v>
+        <v>0.39488368100266769</v>
       </c>
       <c r="L63">
         <v>22</v>
@@ -12872,19 +12862,19 @@
         <v>23299</v>
       </c>
       <c r="G64">
+        <f>F64-B64</f>
+        <v>114</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <f>(F64-B64)/B64</f>
+        <v>4.9169721802889803E-3</v>
+      </c>
+      <c r="J64">
         <f t="shared" si="0"/>
-        <v>114</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="1"/>
-        <v>4.9169721802889803E-3</v>
-      </c>
-      <c r="J64">
-        <f t="shared" si="2"/>
-        <v>100.4916972180289</v>
+        <v>0.49169721802890365</v>
       </c>
       <c r="L64">
         <v>22</v>
@@ -12925,19 +12915,19 @@
         <v>23040</v>
       </c>
       <c r="G65">
-        <f t="shared" si="0"/>
+        <f>F65-B65</f>
         <v>108</v>
       </c>
       <c r="H65">
         <v>1</v>
       </c>
       <c r="I65">
-        <f t="shared" si="1"/>
+        <f>(F65-B65)/B65</f>
         <v>4.7095761381475663E-3</v>
       </c>
       <c r="J65">
-        <f t="shared" si="2"/>
-        <v>100.47095761381476</v>
+        <f t="shared" si="0"/>
+        <v>0.47095761381476109</v>
       </c>
       <c r="L65">
         <v>22</v>
@@ -12978,19 +12968,19 @@
         <v>23012</v>
       </c>
       <c r="G66">
-        <f t="shared" si="0"/>
+        <f>F66-B66</f>
         <v>88</v>
       </c>
       <c r="H66">
         <v>1</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I121" si="3">(F66-B66)/B66</f>
+        <f>(F66-B66)/B66</f>
         <v>3.838771593090211E-3</v>
       </c>
       <c r="J66">
-        <f t="shared" si="2"/>
-        <v>100.38387715930902</v>
+        <f t="shared" si="0"/>
+        <v>0.38387715930902289</v>
       </c>
       <c r="L66">
         <v>22</v>
@@ -13031,19 +13021,19 @@
         <v>23152</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G121" si="4">F67-B67</f>
+        <f>F67-B67</f>
         <v>118</v>
       </c>
       <c r="H67">
         <v>0</v>
       </c>
       <c r="I67">
-        <f t="shared" si="3"/>
+        <f>(F67-B67)/B67</f>
         <v>5.1228618563862113E-3</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J121" si="5">F67*100/B67</f>
-        <v>100.51228618563862</v>
+        <f t="shared" ref="J67:J121" si="1">(F67*100/B67)-100</f>
+        <v>0.51228618563861517</v>
       </c>
       <c r="L67">
         <v>22</v>
@@ -13084,19 +13074,19 @@
         <v>22914</v>
       </c>
       <c r="G68">
-        <f t="shared" si="4"/>
+        <f>F68-B68</f>
         <v>88</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="I68">
-        <f t="shared" si="3"/>
+        <f>(F68-B68)/B68</f>
         <v>3.8552527819153597E-3</v>
       </c>
       <c r="J68">
-        <f t="shared" si="5"/>
-        <v>100.38552527819154</v>
+        <f t="shared" si="1"/>
+        <v>0.38552527819153681</v>
       </c>
       <c r="L68">
         <v>22</v>
@@ -13137,19 +13127,19 @@
         <v>23418</v>
       </c>
       <c r="G69">
-        <f t="shared" si="4"/>
+        <f>F69-B69</f>
         <v>96</v>
       </c>
       <c r="H69">
         <v>1</v>
       </c>
       <c r="I69">
-        <f t="shared" si="3"/>
+        <f>(F69-B69)/B69</f>
         <v>4.1162850527399026E-3</v>
       </c>
       <c r="J69">
-        <f t="shared" si="5"/>
-        <v>100.411628505274</v>
+        <f t="shared" si="1"/>
+        <v>0.41162850527399542</v>
       </c>
       <c r="L69">
         <v>22</v>
@@ -13190,19 +13180,19 @@
         <v>23054</v>
       </c>
       <c r="G70">
-        <f t="shared" si="4"/>
+        <f>F70-B70</f>
         <v>102</v>
       </c>
       <c r="H70">
         <v>1</v>
       </c>
       <c r="I70">
-        <f t="shared" si="3"/>
+        <f>(F70-B70)/B70</f>
         <v>4.4440571627744861E-3</v>
       </c>
       <c r="J70">
-        <f t="shared" si="5"/>
-        <v>100.44440571627744</v>
+        <f t="shared" si="1"/>
+        <v>0.44440571627744418</v>
       </c>
       <c r="L70">
         <v>22</v>
@@ -13243,19 +13233,19 @@
         <v>23117</v>
       </c>
       <c r="G71">
-        <f t="shared" si="4"/>
+        <f>F71-B71</f>
         <v>90</v>
       </c>
       <c r="H71">
         <v>0</v>
       </c>
       <c r="I71">
-        <f t="shared" si="3"/>
+        <f>(F71-B71)/B71</f>
         <v>3.9084552916141919E-3</v>
       </c>
       <c r="J71">
-        <f t="shared" si="5"/>
-        <v>100.39084552916142</v>
+        <f t="shared" si="1"/>
+        <v>0.39084552916142457</v>
       </c>
       <c r="L71">
         <v>22</v>
@@ -13296,19 +13286,19 @@
         <v>22892</v>
       </c>
       <c r="G72">
-        <f t="shared" si="4"/>
+        <f>F72-B72</f>
         <v>50</v>
       </c>
       <c r="H72">
         <v>0</v>
       </c>
       <c r="I72">
-        <f t="shared" si="3"/>
+        <f>(F72-B72)/B72</f>
         <v>2.1889501794939148E-3</v>
       </c>
       <c r="J72">
-        <f t="shared" si="5"/>
-        <v>100.21889501794939</v>
+        <f t="shared" si="1"/>
+        <v>0.21889501794939292</v>
       </c>
       <c r="L72">
         <v>0</v>
@@ -13349,19 +13339,19 @@
         <v>22612</v>
       </c>
       <c r="G73">
-        <f t="shared" si="4"/>
+        <f>F73-B73</f>
         <v>102</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73">
-        <f t="shared" si="3"/>
+        <f>(F73-B73)/B73</f>
         <v>4.5313194135939584E-3</v>
       </c>
       <c r="J73">
-        <f t="shared" si="5"/>
-        <v>100.4531319413594</v>
+        <f t="shared" si="1"/>
+        <v>0.45313194135940194</v>
       </c>
       <c r="L73">
         <v>0</v>
@@ -13402,19 +13392,19 @@
         <v>22997</v>
       </c>
       <c r="G74">
-        <f t="shared" si="4"/>
+        <f>F74-B74</f>
         <v>50</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74">
-        <f t="shared" si="3"/>
+        <f>(F74-B74)/B74</f>
         <v>2.1789340654551795E-3</v>
       </c>
       <c r="J74">
-        <f t="shared" si="5"/>
-        <v>100.21789340654551</v>
+        <f t="shared" si="1"/>
+        <v>0.21789340654551381</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -13455,19 +13445,19 @@
         <v>22219</v>
       </c>
       <c r="G75">
-        <f t="shared" si="4"/>
+        <f>F75-B75</f>
         <v>18</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75">
-        <f t="shared" si="3"/>
+        <f>(F75-B75)/B75</f>
         <v>8.1077428944642137E-4</v>
       </c>
       <c r="J75">
-        <f t="shared" si="5"/>
-        <v>100.08107742894464</v>
+        <f t="shared" si="1"/>
+        <v>8.1077428944638541E-2</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -13508,19 +13498,19 @@
         <v>23270</v>
       </c>
       <c r="G76">
-        <f t="shared" si="4"/>
+        <f>F76-B76</f>
         <v>22</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <f t="shared" si="3"/>
+        <f>(F76-B76)/B76</f>
         <v>9.4631796283551272E-4</v>
       </c>
       <c r="J76">
-        <f t="shared" si="5"/>
-        <v>100.09463179628355</v>
+        <f t="shared" si="1"/>
+        <v>9.4631796283550784E-2</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -13561,19 +13551,19 @@
         <v>22815</v>
       </c>
       <c r="G77">
-        <f t="shared" si="4"/>
+        <f>F77-B77</f>
         <v>70</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <f t="shared" si="3"/>
+        <f>(F77-B77)/B77</f>
         <v>3.0775994724115191E-3</v>
       </c>
       <c r="J77">
-        <f t="shared" si="5"/>
-        <v>100.30775994724115</v>
+        <f t="shared" si="1"/>
+        <v>0.30775994724115208</v>
       </c>
       <c r="L77">
         <v>0</v>
@@ -13614,19 +13604,19 @@
         <v>23025</v>
       </c>
       <c r="G78">
-        <f t="shared" si="4"/>
+        <f>F78-B78</f>
         <v>50</v>
       </c>
       <c r="H78">
         <v>0</v>
       </c>
       <c r="I78">
-        <f t="shared" si="3"/>
+        <f>(F78-B78)/B78</f>
         <v>2.176278563656148E-3</v>
       </c>
       <c r="J78">
-        <f t="shared" si="5"/>
-        <v>100.21762785636561</v>
+        <f t="shared" si="1"/>
+        <v>0.21762785636560977</v>
       </c>
       <c r="L78">
         <v>0</v>
@@ -13667,19 +13657,19 @@
         <v>22570</v>
       </c>
       <c r="G79">
-        <f t="shared" si="4"/>
+        <f>F79-B79</f>
         <v>100</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
       <c r="I79">
-        <f t="shared" si="3"/>
+        <f>(F79-B79)/B79</f>
         <v>4.450378282153983E-3</v>
       </c>
       <c r="J79">
-        <f t="shared" si="5"/>
-        <v>100.4450378282154</v>
+        <f t="shared" si="1"/>
+        <v>0.44503782821540483</v>
       </c>
       <c r="L79">
         <v>0</v>
@@ -13720,19 +13710,19 @@
         <v>23109</v>
       </c>
       <c r="G80">
-        <f t="shared" si="4"/>
+        <f>F80-B80</f>
         <v>50</v>
       </c>
       <c r="H80">
         <v>1</v>
       </c>
       <c r="I80">
-        <f t="shared" si="3"/>
+        <f>(F80-B80)/B80</f>
         <v>2.1683507524177109E-3</v>
       </c>
       <c r="J80">
-        <f t="shared" si="5"/>
-        <v>100.21683507524178</v>
+        <f t="shared" si="1"/>
+        <v>0.21683507524177514</v>
       </c>
       <c r="L80">
         <v>0</v>
@@ -13773,19 +13763,19 @@
         <v>22591</v>
       </c>
       <c r="G81">
-        <f t="shared" si="4"/>
+        <f>F81-B81</f>
         <v>88</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81">
-        <f t="shared" si="3"/>
+        <f>(F81-B81)/B81</f>
         <v>3.9105896991512247E-3</v>
       </c>
       <c r="J81">
-        <f t="shared" si="5"/>
-        <v>100.39105896991512</v>
+        <f t="shared" si="1"/>
+        <v>0.39105896991512168</v>
       </c>
       <c r="L81">
         <v>0</v>
@@ -13826,19 +13816,19 @@
         <v>49556</v>
       </c>
       <c r="G82">
-        <f t="shared" si="4"/>
+        <f>F82-B82</f>
         <v>146</v>
       </c>
       <c r="H82">
         <v>1</v>
       </c>
       <c r="I82">
-        <f t="shared" si="3"/>
+        <f>(F82-B82)/B82</f>
         <v>2.9548674357417525E-3</v>
       </c>
       <c r="J82">
-        <f t="shared" si="5"/>
-        <v>100.29548674357417</v>
+        <f t="shared" si="1"/>
+        <v>0.29548674357417326</v>
       </c>
       <c r="L82">
         <v>44</v>
@@ -13879,19 +13869,19 @@
         <v>48411</v>
       </c>
       <c r="G83">
-        <f t="shared" si="4"/>
+        <f>F83-B83</f>
         <v>70</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83">
-        <f t="shared" si="3"/>
+        <f>(F83-B83)/B83</f>
         <v>1.4480461719865124E-3</v>
       </c>
       <c r="J83">
-        <f t="shared" si="5"/>
-        <v>100.14480461719864</v>
+        <f t="shared" si="1"/>
+        <v>0.14480461719864479</v>
       </c>
       <c r="L83">
         <v>42</v>
@@ -13932,19 +13922,19 @@
         <v>49092</v>
       </c>
       <c r="G84">
-        <f t="shared" si="4"/>
+        <f>F84-B84</f>
         <v>152</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84">
-        <f t="shared" si="3"/>
+        <f>(F84-B84)/B84</f>
         <v>3.1058438904781366E-3</v>
       </c>
       <c r="J84">
-        <f t="shared" si="5"/>
-        <v>100.31058438904782</v>
+        <f t="shared" si="1"/>
+        <v>0.31058438904781838</v>
       </c>
       <c r="L84">
         <v>43</v>
@@ -13985,19 +13975,19 @@
         <v>48201</v>
       </c>
       <c r="G85">
-        <f t="shared" si="4"/>
+        <f>F85-B85</f>
         <v>80</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85">
-        <f t="shared" si="3"/>
+        <f>(F85-B85)/B85</f>
         <v>1.6624758421479187E-3</v>
       </c>
       <c r="J85">
-        <f t="shared" si="5"/>
-        <v>100.16624758421479</v>
+        <f t="shared" si="1"/>
+        <v>0.16624758421478703</v>
       </c>
       <c r="L85">
         <v>42</v>
@@ -14038,19 +14028,19 @@
         <v>48264</v>
       </c>
       <c r="G86">
-        <f t="shared" si="4"/>
+        <f>F86-B86</f>
         <v>102</v>
       </c>
       <c r="H86">
         <v>2</v>
       </c>
       <c r="I86">
-        <f t="shared" si="3"/>
+        <f>(F86-B86)/B86</f>
         <v>2.1178522486607699E-3</v>
       </c>
       <c r="J86">
-        <f t="shared" si="5"/>
-        <v>100.21178522486608</v>
+        <f t="shared" si="1"/>
+        <v>0.21178522486607676</v>
       </c>
       <c r="L86">
         <v>42</v>
@@ -14091,19 +14081,19 @@
         <v>48805</v>
       </c>
       <c r="G87">
-        <f t="shared" si="4"/>
+        <f>F87-B87</f>
         <v>124</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
       <c r="I87">
-        <f t="shared" si="3"/>
+        <f>(F87-B87)/B87</f>
         <v>2.5471950042110884E-3</v>
       </c>
       <c r="J87">
-        <f t="shared" si="5"/>
-        <v>100.2547195004211</v>
+        <f t="shared" si="1"/>
+        <v>0.25471950042110336</v>
       </c>
       <c r="L87">
         <v>43</v>
@@ -14144,19 +14134,19 @@
         <v>48784</v>
       </c>
       <c r="G88">
-        <f t="shared" si="4"/>
+        <f>F88-B88</f>
         <v>104</v>
       </c>
       <c r="H88">
         <v>1</v>
       </c>
       <c r="I88">
-        <f t="shared" si="3"/>
+        <f>(F88-B88)/B88</f>
         <v>2.1364009860312242E-3</v>
       </c>
       <c r="J88">
-        <f t="shared" si="5"/>
-        <v>100.21364009860312</v>
+        <f t="shared" si="1"/>
+        <v>0.21364009860312194</v>
       </c>
       <c r="L88">
         <v>43</v>
@@ -14197,19 +14187,19 @@
         <v>47998</v>
       </c>
       <c r="G89">
-        <f t="shared" si="4"/>
+        <f>F89-B89</f>
         <v>116</v>
       </c>
       <c r="H89">
         <v>1</v>
       </c>
       <c r="I89">
-        <f t="shared" si="3"/>
+        <f>(F89-B89)/B89</f>
         <v>2.422622279771104E-3</v>
       </c>
       <c r="J89">
-        <f t="shared" si="5"/>
-        <v>100.24226222797711</v>
+        <f t="shared" si="1"/>
+        <v>0.24226222797710761</v>
       </c>
       <c r="L89">
         <v>42</v>
@@ -14250,19 +14240,19 @@
         <v>48278</v>
       </c>
       <c r="G90">
-        <f t="shared" si="4"/>
+        <f>F90-B90</f>
         <v>100</v>
       </c>
       <c r="H90">
         <v>2</v>
       </c>
       <c r="I90">
-        <f t="shared" si="3"/>
+        <f>(F90-B90)/B90</f>
         <v>2.0756361824899329E-3</v>
       </c>
       <c r="J90">
-        <f t="shared" si="5"/>
-        <v>100.207563618249</v>
+        <f t="shared" si="1"/>
+        <v>0.20756361824899727</v>
       </c>
       <c r="L90">
         <v>42</v>
@@ -14303,19 +14293,19 @@
         <v>47758</v>
       </c>
       <c r="G91">
-        <f t="shared" si="4"/>
+        <f>F91-B91</f>
         <v>26</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <f t="shared" si="3"/>
+        <f>(F91-B91)/B91</f>
         <v>5.4470795273610991E-4</v>
       </c>
       <c r="J91">
-        <f t="shared" si="5"/>
-        <v>100.05447079527362</v>
+        <f t="shared" si="1"/>
+        <v>5.4470795273616091E-2</v>
       </c>
       <c r="L91">
         <v>41</v>
@@ -14356,19 +14346,19 @@
         <v>46296</v>
       </c>
       <c r="G92">
-        <f t="shared" si="4"/>
+        <f>F92-B92</f>
         <v>22</v>
       </c>
       <c r="H92">
         <v>1</v>
       </c>
       <c r="I92">
-        <f t="shared" si="3"/>
+        <f>(F92-B92)/B92</f>
         <v>4.7542896659030987E-4</v>
       </c>
       <c r="J92">
-        <f t="shared" si="5"/>
-        <v>100.04754289665902</v>
+        <f t="shared" si="1"/>
+        <v>4.7542896659024336E-2</v>
       </c>
       <c r="L92">
         <v>0</v>
@@ -14409,19 +14399,19 @@
         <v>47529</v>
       </c>
       <c r="G93">
-        <f t="shared" si="4"/>
+        <f>F93-B93</f>
         <v>30</v>
       </c>
       <c r="H93">
         <v>2</v>
       </c>
       <c r="I93">
-        <f t="shared" si="3"/>
+        <f>(F93-B93)/B93</f>
         <v>6.3159224404724307E-4</v>
       </c>
       <c r="J93">
-        <f t="shared" si="5"/>
-        <v>100.06315922440473</v>
+        <f t="shared" si="1"/>
+        <v>6.315922440472832E-2</v>
       </c>
       <c r="L93">
         <v>0</v>
@@ -14462,19 +14452,19 @@
         <v>47200</v>
       </c>
       <c r="G94">
-        <f t="shared" si="4"/>
+        <f>F94-B94</f>
         <v>20</v>
       </c>
       <c r="H94">
         <v>2</v>
       </c>
       <c r="I94">
-        <f t="shared" si="3"/>
+        <f>(F94-B94)/B94</f>
         <v>4.2390843577787198E-4</v>
       </c>
       <c r="J94">
-        <f t="shared" si="5"/>
-        <v>100.04239084357779</v>
+        <f t="shared" si="1"/>
+        <v>4.239084357779177E-2</v>
       </c>
       <c r="L94">
         <v>0</v>
@@ -14515,19 +14505,19 @@
         <v>48636</v>
       </c>
       <c r="G95">
-        <f t="shared" si="4"/>
+        <f>F95-B95</f>
         <v>0</v>
       </c>
       <c r="H95">
         <v>2</v>
       </c>
       <c r="I95">
-        <f t="shared" si="3"/>
+        <f>(F95-B95)/B95</f>
         <v>0</v>
       </c>
       <c r="J95">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L95">
         <v>0</v>
@@ -14568,19 +14558,19 @@
         <v>48405</v>
       </c>
       <c r="G96">
-        <f t="shared" si="4"/>
+        <f>F96-B96</f>
         <v>30</v>
       </c>
       <c r="H96">
         <v>2</v>
       </c>
       <c r="I96">
-        <f t="shared" si="3"/>
+        <f>(F96-B96)/B96</f>
         <v>6.2015503875968996E-4</v>
       </c>
       <c r="J96">
-        <f t="shared" si="5"/>
-        <v>100.06201550387597</v>
+        <f t="shared" si="1"/>
+        <v>6.2015503875969102E-2</v>
       </c>
       <c r="L96">
         <v>0</v>
@@ -14621,19 +14611,19 @@
         <v>48027</v>
       </c>
       <c r="G97">
-        <f t="shared" si="4"/>
+        <f>F97-B97</f>
         <v>100</v>
       </c>
       <c r="H97">
         <v>1</v>
       </c>
       <c r="I97">
-        <f t="shared" si="3"/>
+        <f>(F97-B97)/B97</f>
         <v>2.0865065620631375E-3</v>
       </c>
       <c r="J97">
-        <f t="shared" si="5"/>
-        <v>100.20865065620632</v>
+        <f t="shared" si="1"/>
+        <v>0.2086506562063164</v>
       </c>
       <c r="L97">
         <v>0</v>
@@ -14674,19 +14664,19 @@
         <v>48020</v>
       </c>
       <c r="G98">
-        <f t="shared" si="4"/>
+        <f>F98-B98</f>
         <v>100</v>
       </c>
       <c r="H98">
         <v>1</v>
       </c>
       <c r="I98">
-        <f t="shared" si="3"/>
+        <f>(F98-B98)/B98</f>
         <v>2.0868113522537562E-3</v>
       </c>
       <c r="J98">
-        <f t="shared" si="5"/>
-        <v>100.20868113522538</v>
+        <f t="shared" si="1"/>
+        <v>0.20868113522537612</v>
       </c>
       <c r="L98">
         <v>0</v>
@@ -14727,19 +14717,19 @@
         <v>48167</v>
       </c>
       <c r="G99">
-        <f t="shared" si="4"/>
+        <f>F99-B99</f>
         <v>56</v>
       </c>
       <c r="H99">
         <v>0</v>
       </c>
       <c r="I99">
-        <f t="shared" si="3"/>
+        <f>(F99-B99)/B99</f>
         <v>1.1639749745380474E-3</v>
       </c>
       <c r="J99">
-        <f t="shared" si="5"/>
-        <v>100.1163974974538</v>
+        <f t="shared" si="1"/>
+        <v>0.11639749745380357</v>
       </c>
       <c r="L99">
         <v>0</v>
@@ -14780,19 +14770,19 @@
         <v>47158</v>
       </c>
       <c r="G100">
-        <f t="shared" si="4"/>
+        <f>F100-B100</f>
         <v>30</v>
       </c>
       <c r="H100">
         <v>2</v>
       </c>
       <c r="I100">
-        <f t="shared" si="3"/>
+        <f>(F100-B100)/B100</f>
         <v>6.3656425055168904E-4</v>
       </c>
       <c r="J100">
-        <f t="shared" si="5"/>
-        <v>100.06365642505517</v>
+        <f t="shared" si="1"/>
+        <v>6.3656425055171439E-2</v>
       </c>
       <c r="L100">
         <v>0</v>
@@ -14833,19 +14823,19 @@
         <v>47480</v>
       </c>
       <c r="G101">
-        <f t="shared" si="4"/>
+        <f>F101-B101</f>
         <v>6</v>
       </c>
       <c r="H101">
         <v>1</v>
       </c>
       <c r="I101">
-        <f t="shared" si="3"/>
+        <f>(F101-B101)/B101</f>
         <v>1.2638496861439946E-4</v>
       </c>
       <c r="J101">
-        <f t="shared" si="5"/>
-        <v>100.01263849686144</v>
+        <f t="shared" si="1"/>
+        <v>1.2638496861441695E-2</v>
       </c>
       <c r="L101">
         <v>0</v>
@@ -14886,19 +14876,19 @@
         <v>57808</v>
       </c>
       <c r="G102">
-        <f t="shared" si="4"/>
+        <f>F102-B102</f>
         <v>76</v>
       </c>
       <c r="H102">
         <v>1</v>
       </c>
       <c r="I102">
-        <f t="shared" si="3"/>
+        <f>(F102-B102)/B102</f>
         <v>1.3164276311231206E-3</v>
       </c>
       <c r="J102">
-        <f t="shared" si="5"/>
-        <v>100.13164276311231</v>
+        <f t="shared" si="1"/>
+        <v>0.13164276311231049</v>
       </c>
       <c r="L102">
         <v>54</v>
@@ -14939,19 +14929,19 @@
         <v>57997</v>
       </c>
       <c r="G103">
-        <f t="shared" si="4"/>
+        <f>F103-B103</f>
         <v>176</v>
       </c>
       <c r="H103">
         <v>1</v>
       </c>
       <c r="I103">
-        <f t="shared" si="3"/>
+        <f>(F103-B103)/B103</f>
         <v>3.0438767921689351E-3</v>
       </c>
       <c r="J103">
-        <f t="shared" si="5"/>
-        <v>100.30438767921689</v>
+        <f t="shared" si="1"/>
+        <v>0.30438767921688736</v>
       </c>
       <c r="L103">
         <v>54</v>
@@ -14992,19 +14982,19 @@
         <v>58046</v>
       </c>
       <c r="G104">
-        <f t="shared" si="4"/>
+        <f>F104-B104</f>
         <v>6</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <f t="shared" si="3"/>
+        <f>(F104-B104)/B104</f>
         <v>1.0337698139214335E-4</v>
       </c>
       <c r="J104">
-        <f t="shared" si="5"/>
-        <v>100.01033769813921</v>
+        <f t="shared" si="1"/>
+        <v>1.0337698139210261E-2</v>
       </c>
       <c r="L104">
         <v>54</v>
@@ -15045,19 +15035,19 @@
         <v>58559</v>
       </c>
       <c r="G105">
-        <f t="shared" si="4"/>
+        <f>F105-B105</f>
         <v>44</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <f t="shared" si="3"/>
+        <f>(F105-B105)/B105</f>
         <v>7.5194394599675297E-4</v>
       </c>
       <c r="J105">
-        <f t="shared" si="5"/>
-        <v>100.07519439459968</v>
+        <f t="shared" si="1"/>
+        <v>7.5194394599677139E-2</v>
       </c>
       <c r="L105">
         <v>55</v>
@@ -15098,19 +15088,19 @@
         <v>58384</v>
       </c>
       <c r="G106">
-        <f t="shared" si="4"/>
+        <f>F106-B106</f>
         <v>168</v>
       </c>
       <c r="H106">
         <v>1</v>
       </c>
       <c r="I106">
-        <f t="shared" si="3"/>
+        <f>(F106-B106)/B106</f>
         <v>2.8858045898034904E-3</v>
       </c>
       <c r="J106">
-        <f t="shared" si="5"/>
-        <v>100.28858045898035</v>
+        <f t="shared" si="1"/>
+        <v>0.28858045898034845</v>
       </c>
       <c r="L106">
         <v>55</v>
@@ -15151,19 +15141,19 @@
         <v>57773</v>
       </c>
       <c r="G107">
-        <f t="shared" si="4"/>
+        <f>F107-B107</f>
         <v>108</v>
       </c>
       <c r="H107">
         <v>1</v>
       </c>
       <c r="I107">
-        <f t="shared" si="3"/>
+        <f>(F107-B107)/B107</f>
         <v>1.8728864996098154E-3</v>
       </c>
       <c r="J107">
-        <f t="shared" si="5"/>
-        <v>100.18728864996098</v>
+        <f t="shared" si="1"/>
+        <v>0.18728864996097627</v>
       </c>
       <c r="L107">
         <v>54</v>
@@ -15204,19 +15194,19 @@
         <v>57724</v>
       </c>
       <c r="G108">
-        <f t="shared" si="4"/>
+        <f>F108-B108</f>
         <v>124</v>
       </c>
       <c r="H108">
         <v>0</v>
       </c>
       <c r="I108">
-        <f t="shared" si="3"/>
+        <f>(F108-B108)/B108</f>
         <v>2.1527777777777778E-3</v>
       </c>
       <c r="J108">
-        <f t="shared" si="5"/>
-        <v>100.21527777777777</v>
+        <f t="shared" si="1"/>
+        <v>0.21527777777777146</v>
       </c>
       <c r="L108">
         <v>54</v>
@@ -15257,19 +15247,19 @@
         <v>58370</v>
       </c>
       <c r="G109">
-        <f t="shared" si="4"/>
+        <f>F109-B109</f>
         <v>108</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109">
-        <f t="shared" si="3"/>
+        <f>(F109-B109)/B109</f>
         <v>1.8536953760598675E-3</v>
       </c>
       <c r="J109">
-        <f t="shared" si="5"/>
-        <v>100.18536953760599</v>
+        <f t="shared" si="1"/>
+        <v>0.18536953760599317</v>
       </c>
       <c r="L109">
         <v>55</v>
@@ -15310,19 +15300,19 @@
         <v>58067</v>
       </c>
       <c r="G110">
-        <f t="shared" si="4"/>
+        <f>F110-B110</f>
         <v>46</v>
       </c>
       <c r="H110">
         <v>1</v>
       </c>
       <c r="I110">
-        <f t="shared" si="3"/>
+        <f>(F110-B110)/B110</f>
         <v>7.9281639406421811E-4</v>
       </c>
       <c r="J110">
-        <f t="shared" si="5"/>
-        <v>100.07928163940642</v>
+        <f t="shared" si="1"/>
+        <v>7.9281639406417526E-2</v>
       </c>
       <c r="L110">
         <v>54</v>
@@ -15363,19 +15353,19 @@
         <v>58573</v>
       </c>
       <c r="G111">
-        <f t="shared" si="4"/>
+        <f>F111-B111</f>
         <v>188</v>
       </c>
       <c r="H111">
         <v>1</v>
       </c>
       <c r="I111">
-        <f t="shared" si="3"/>
+        <f>(F111-B111)/B111</f>
         <v>3.2200051383060716E-3</v>
       </c>
       <c r="J111">
-        <f t="shared" si="5"/>
-        <v>100.3220005138306</v>
+        <f t="shared" si="1"/>
+        <v>0.32200051383060213</v>
       </c>
       <c r="L111">
         <v>55</v>
@@ -15416,19 +15406,19 @@
         <v>57520</v>
       </c>
       <c r="G112">
-        <f t="shared" si="4"/>
+        <f>F112-B112</f>
         <v>-6</v>
       </c>
       <c r="H112">
         <v>1</v>
       </c>
       <c r="I112">
-        <f t="shared" si="3"/>
+        <f>(F112-B112)/B112</f>
         <v>-1.0430066404756111E-4</v>
       </c>
       <c r="J112">
-        <f t="shared" si="5"/>
-        <v>99.989569933595249</v>
+        <f t="shared" si="1"/>
+        <v>-1.0430066404751415E-2</v>
       </c>
       <c r="L112">
         <v>0</v>
@@ -15469,19 +15459,19 @@
         <v>57324</v>
       </c>
       <c r="G113">
-        <f t="shared" si="4"/>
+        <f>F113-B113</f>
         <v>-138</v>
       </c>
       <c r="H113">
         <v>2</v>
       </c>
       <c r="I113">
-        <f t="shared" si="3"/>
+        <f>(F113-B113)/B113</f>
         <v>-2.4015871358462984E-3</v>
       </c>
       <c r="J113">
-        <f t="shared" si="5"/>
-        <v>99.759841286415366</v>
+        <f t="shared" si="1"/>
+        <v>-0.24015871358463414</v>
       </c>
       <c r="L113">
         <v>0</v>
@@ -15522,19 +15512,19 @@
         <v>56784</v>
       </c>
       <c r="G114">
-        <f t="shared" si="4"/>
+        <f>F114-B114</f>
         <v>16</v>
       </c>
       <c r="H114">
         <v>1</v>
       </c>
       <c r="I114">
-        <f t="shared" si="3"/>
+        <f>(F114-B114)/B114</f>
         <v>2.8184892897406989E-4</v>
       </c>
       <c r="J114">
-        <f t="shared" si="5"/>
-        <v>100.0281848928974</v>
+        <f t="shared" si="1"/>
+        <v>2.8184892897400005E-2</v>
       </c>
       <c r="L114">
         <v>0</v>
@@ -15575,19 +15565,19 @@
         <v>56686</v>
       </c>
       <c r="G115">
-        <f t="shared" si="4"/>
+        <f>F115-B115</f>
         <v>-32</v>
       </c>
       <c r="H115">
         <v>2</v>
       </c>
       <c r="I115">
-        <f t="shared" si="3"/>
+        <f>(F115-B115)/B115</f>
         <v>-5.6419478825064354E-4</v>
       </c>
       <c r="J115">
-        <f t="shared" si="5"/>
-        <v>99.943580521174937</v>
+        <f t="shared" si="1"/>
+        <v>-5.6419478825063152E-2</v>
       </c>
       <c r="L115">
         <v>0</v>
@@ -15628,19 +15618,19 @@
         <v>56980</v>
       </c>
       <c r="G116">
-        <f t="shared" si="4"/>
+        <f>F116-B116</f>
         <v>12</v>
       </c>
       <c r="H116">
         <v>0</v>
       </c>
       <c r="I116">
-        <f t="shared" si="3"/>
+        <f>(F116-B116)/B116</f>
         <v>2.1064457239151804E-4</v>
       </c>
       <c r="J116">
-        <f t="shared" si="5"/>
-        <v>100.02106445723915</v>
+        <f t="shared" si="1"/>
+        <v>2.1064457239148737E-2</v>
       </c>
       <c r="L116">
         <v>0</v>
@@ -15681,19 +15671,19 @@
         <v>57064</v>
       </c>
       <c r="G117">
-        <f t="shared" si="4"/>
+        <f>F117-B117</f>
         <v>-20</v>
       </c>
       <c r="H117">
         <v>2</v>
       </c>
       <c r="I117">
-        <f t="shared" si="3"/>
+        <f>(F117-B117)/B117</f>
         <v>-3.503608716978488E-4</v>
       </c>
       <c r="J117">
-        <f t="shared" si="5"/>
-        <v>99.964963912830214</v>
+        <f t="shared" si="1"/>
+        <v>-3.5036087169785901E-2</v>
       </c>
       <c r="L117">
         <v>0</v>
@@ -15734,19 +15724,19 @@
         <v>56567</v>
       </c>
       <c r="G118">
-        <f t="shared" si="4"/>
+        <f>F118-B118</f>
         <v>10</v>
       </c>
       <c r="H118">
         <v>1</v>
       </c>
       <c r="I118">
-        <f t="shared" si="3"/>
+        <f>(F118-B118)/B118</f>
         <v>1.7681277295471826E-4</v>
       </c>
       <c r="J118">
-        <f t="shared" si="5"/>
-        <v>100.01768127729547</v>
+        <f t="shared" si="1"/>
+        <v>1.7681277295466202E-2</v>
       </c>
       <c r="L118">
         <v>0</v>
@@ -15787,19 +15777,19 @@
         <v>56973</v>
       </c>
       <c r="G119">
-        <f t="shared" si="4"/>
+        <f>F119-B119</f>
         <v>-50</v>
       </c>
       <c r="H119">
         <v>1</v>
       </c>
       <c r="I119">
-        <f t="shared" si="3"/>
+        <f>(F119-B119)/B119</f>
         <v>-8.7683917015940937E-4</v>
       </c>
       <c r="J119">
-        <f t="shared" si="5"/>
-        <v>99.912316082984063</v>
+        <f t="shared" si="1"/>
+        <v>-8.7683917015937141E-2</v>
       </c>
       <c r="L119">
         <v>0</v>
@@ -15840,19 +15830,19 @@
         <v>57716</v>
       </c>
       <c r="G120">
-        <f t="shared" si="4"/>
+        <f>F120-B120</f>
         <v>-40</v>
       </c>
       <c r="H120">
         <v>0</v>
       </c>
       <c r="I120">
-        <f t="shared" si="3"/>
+        <f>(F120-B120)/B120</f>
         <v>-6.925687374471916E-4</v>
       </c>
       <c r="J120">
-        <f t="shared" si="5"/>
-        <v>99.93074312625528</v>
+        <f t="shared" si="1"/>
+        <v>-6.9256873744720338E-2</v>
       </c>
       <c r="L120">
         <v>0</v>
@@ -15893,19 +15883,19 @@
         <v>56203</v>
       </c>
       <c r="G121">
-        <f t="shared" si="4"/>
+        <f>F121-B121</f>
         <v>-60</v>
       </c>
       <c r="H121">
         <v>1</v>
       </c>
       <c r="I121">
-        <f t="shared" si="3"/>
+        <f>(F121-B121)/B121</f>
         <v>-1.0664202051081527E-3</v>
       </c>
       <c r="J121">
-        <f t="shared" si="5"/>
-        <v>99.893357979489181</v>
+        <f t="shared" si="1"/>
+        <v>-0.10664202051081872</v>
       </c>
       <c r="L121">
         <v>0</v>
@@ -15948,7 +15938,7 @@
       </c>
       <c r="J124">
         <f>SUM(J2:J121)/120</f>
-        <v>99.642931325294867</v>
+        <v>-0.35706867470510051</v>
       </c>
     </row>
   </sheetData>
@@ -21476,7 +21466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>